<commit_message>
update setting rencana bonvoyage
</commit_message>
<xml_diff>
--- a/RENCANA BON VOYAGE.xlsx
+++ b/RENCANA BON VOYAGE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mapan\progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C75E790D-2182-4670-9BC4-DFE6C3ACB9AA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12211A1F-DB19-4443-85E7-AA09BAE2D5CE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="16080" windowWidth="29040" windowHeight="7965" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,9 +30,6 @@
     <t>KELAS</t>
   </si>
   <si>
-    <t>ANGKATAN</t>
-  </si>
-  <si>
     <t>JUMLAH</t>
   </si>
   <si>
@@ -238,6 +235,9 @@
   </si>
   <si>
     <t>HALILINTAR</t>
+  </si>
+  <si>
+    <t>ANGK.</t>
   </si>
 </sst>
 </file>
@@ -678,19 +678,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="20.42578125" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.85546875" customWidth="1"/>
-    <col min="5" max="5" width="24" customWidth="1"/>
-    <col min="6" max="6" width="21.28515625" customWidth="1"/>
-    <col min="7" max="7" width="23.85546875" customWidth="1"/>
-    <col min="8" max="8" width="20" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
@@ -701,22 +702,22 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="H1" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -724,25 +725,25 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" s="3">
         <v>8</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>13</v>
-      </c>
       <c r="H2" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -751,13 +752,13 @@
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H3" s="3"/>
     </row>
@@ -766,25 +767,25 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="3">
+        <v>8</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="3">
-        <v>8</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>17</v>
-      </c>
       <c r="E4" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -793,13 +794,13 @@
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H5" s="3"/>
     </row>
@@ -818,20 +819,20 @@
         <v>3</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" s="3">
         <v>9</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H7" s="5">
         <v>44444</v>
@@ -843,7 +844,7 @@
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3">
@@ -869,20 +870,20 @@
         <v>4</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10" s="3">
         <v>9</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H10" s="5">
         <v>44444</v>
@@ -894,7 +895,7 @@
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3">
@@ -917,23 +918,23 @@
         <v>5</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C13" s="3">
         <v>15</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="H13" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
@@ -942,7 +943,7 @@
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="3">
@@ -965,23 +966,23 @@
         <v>6</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C16" s="3">
         <v>15</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F16" s="3"/>
       <c r="G16" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -990,7 +991,7 @@
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3">
@@ -1013,20 +1014,20 @@
         <v>7</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C19" s="3">
         <v>16</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H19" s="5">
         <v>44520</v>
@@ -1038,7 +1039,7 @@
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F20" s="3"/>
       <c r="G20" s="3">
@@ -1061,20 +1062,20 @@
         <v>8</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C22" s="3">
         <v>16</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F22" s="3"/>
       <c r="G22" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H22" s="5">
         <v>44520</v>
@@ -1086,7 +1087,7 @@
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F23" s="3"/>
       <c r="G23" s="3">
@@ -1109,25 +1110,25 @@
         <v>9</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C25" s="3">
         <v>29</v>
       </c>
       <c r="D25" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H25" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="H25" s="3" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -1145,19 +1146,19 @@
         <v>10</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C27" s="3">
         <v>30</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
@@ -1168,14 +1169,14 @@
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F28" s="3"/>
       <c r="G28" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -1193,20 +1194,20 @@
         <v>11</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C30" s="3">
         <v>31</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F30" s="3"/>
       <c r="G30" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H30" s="5">
         <v>44501</v>
@@ -1218,7 +1219,7 @@
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
       <c r="E31" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F31" s="3"/>
       <c r="G31" s="3">
@@ -1241,25 +1242,25 @@
         <v>12</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C33" s="3">
         <v>24</v>
       </c>
       <c r="D33" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F33" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E33" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F33" s="3" t="s">
+      <c r="G33" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="G33" s="3" t="s">
+      <c r="H33" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="H33" s="3" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -1277,22 +1278,22 @@
         <v>13</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C35" s="3">
         <v>25</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H35" s="5">
         <v>44501</v>
@@ -1304,7 +1305,7 @@
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
       <c r="E36" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
@@ -1325,22 +1326,22 @@
         <v>14</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C38" s="3">
         <v>31</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H38" s="3"/>
     </row>
@@ -1350,12 +1351,12 @@
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
       <c r="E39" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
       <c r="H39" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -1373,23 +1374,23 @@
         <v>15</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C41" s="3">
         <v>32</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F41" s="3"/>
       <c r="G41" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="H41" s="3" t="s">
         <v>66</v>
-      </c>
-      <c r="H41" s="3" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -1398,7 +1399,7 @@
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
       <c r="E42" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F42" s="3"/>
       <c r="G42" s="3">
@@ -1421,20 +1422,20 @@
         <v>16</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C44" s="8">
         <v>27</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E44" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F44" s="8"/>
       <c r="G44" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H44" s="9">
         <v>44409</v>
@@ -1446,7 +1447,7 @@
       <c r="C45" s="8"/>
       <c r="D45" s="8"/>
       <c r="E45" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F45" s="8"/>
       <c r="G45" s="8"/>
@@ -1467,23 +1468,23 @@
         <v>17</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C47" s="3">
         <v>38</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F47" s="3"/>
       <c r="G47" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H47" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -1492,7 +1493,7 @@
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
       <c r="E48" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F48" s="3"/>
       <c r="G48" s="3"/>
@@ -1513,23 +1514,23 @@
         <v>18</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C50" s="3">
         <v>38</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F50" s="3"/>
       <c r="G50" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I50" s="6"/>
       <c r="J50" s="7"/>
@@ -1542,7 +1543,7 @@
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
       <c r="E51" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F51" s="3"/>
       <c r="G51" s="3"/>
@@ -1563,20 +1564,20 @@
         <v>19</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C53" s="3">
         <v>39</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F53" s="3"/>
       <c r="G53" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H53" s="5">
         <v>44444</v>
@@ -1588,7 +1589,7 @@
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
       <c r="E54" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F54" s="3"/>
       <c r="G54" s="3">
@@ -1611,20 +1612,20 @@
         <v>20</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C56" s="3">
         <v>39</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F56" s="3"/>
       <c r="G56" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H56" s="5">
         <v>44444</v>
@@ -1636,7 +1637,7 @@
       <c r="C57" s="3"/>
       <c r="D57" s="3"/>
       <c r="E57" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F57" s="3"/>
       <c r="G57" s="3">
@@ -1706,7 +1707,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="81" orientation="portrait" r:id="rId1"/>
+  <colBreaks count="1" manualBreakCount="1">
+    <brk id="8" max="1048575" man="1"/>
+  </colBreaks>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
cetak label susulan taruna
</commit_message>
<xml_diff>
--- a/RENCANA BON VOYAGE.xlsx
+++ b/RENCANA BON VOYAGE.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24131"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mapan\progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{110AE6C0-D709-448C-8B6B-00D5BFBFF567}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F266D5B-9B14-4FDB-812C-54D07E2FCB0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="117">
   <si>
     <t>NO</t>
   </si>
@@ -358,13 +358,25 @@
     <t>24 juni</t>
   </si>
   <si>
-    <t>dana masuk</t>
-  </si>
-  <si>
     <t>MAULANA AINUL YAQIN</t>
   </si>
   <si>
     <t>22 maret 22</t>
+  </si>
+  <si>
+    <t>18 ORANG</t>
+  </si>
+  <si>
+    <t>06 JULI</t>
+  </si>
+  <si>
+    <t>21 JULI</t>
+  </si>
+  <si>
+    <t>ABD. ROHMAN</t>
+  </si>
+  <si>
+    <t>01 DES 21</t>
   </si>
 </sst>
 </file>
@@ -486,7 +498,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -584,6 +596,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -924,10 +939,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:O79"/>
+  <dimension ref="A1:O67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="H61" sqref="H61"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="F66" sqref="F66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2023,18 +2038,20 @@
       <c r="C60" s="8">
         <v>26</v>
       </c>
-      <c r="D60" s="8"/>
+      <c r="D60" s="8" t="s">
+        <v>48</v>
+      </c>
       <c r="E60" s="8" t="s">
         <v>7</v>
       </c>
       <c r="F60" s="8" t="s">
-        <v>86</v>
+        <v>113</v>
       </c>
       <c r="G60" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="H60" s="9" t="s">
         <v>111</v>
-      </c>
-      <c r="H60" s="9" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.2">
@@ -2062,115 +2079,80 @@
       <c r="H62" s="10"/>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A63" s="10"/>
-      <c r="B63" s="10"/>
-      <c r="C63" s="10"/>
-      <c r="D63" s="10"/>
-      <c r="E63" s="10"/>
-      <c r="F63" s="10"/>
-      <c r="G63" s="10"/>
-      <c r="H63" s="10"/>
+      <c r="A63" s="38">
+        <v>22</v>
+      </c>
+      <c r="B63" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C63" s="8">
+        <v>28</v>
+      </c>
+      <c r="D63" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="E63" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F63" s="38" t="s">
+        <v>114</v>
+      </c>
+      <c r="G63" s="38" t="s">
+        <v>115</v>
+      </c>
+      <c r="H63" s="38" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A64" s="10"/>
       <c r="B64" s="10"/>
-      <c r="C64" s="10"/>
+      <c r="C64" s="8"/>
       <c r="D64" s="10"/>
-      <c r="E64" s="10"/>
-      <c r="F64" s="10"/>
-      <c r="G64" s="10"/>
-      <c r="H64" s="10"/>
-    </row>
-    <row r="68" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D68" s="35" t="s">
-        <v>9</v>
-      </c>
-      <c r="E68" s="7">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="69" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D69" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="E69" s="7">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="70" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D70" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="E70" s="7">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="71" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D71" s="8" t="s">
+      <c r="E64" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F64" s="38"/>
+      <c r="G64" s="38">
+        <v>85649115380</v>
+      </c>
+      <c r="H64" s="38"/>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A65" s="38"/>
+      <c r="B65" s="10"/>
+      <c r="C65" s="8"/>
+      <c r="D65" s="10"/>
+      <c r="E65" s="8"/>
+      <c r="F65" s="38"/>
+      <c r="G65" s="38"/>
+      <c r="H65" s="38"/>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A66" s="10">
         <v>23</v>
       </c>
-      <c r="E71" s="7">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="72" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D72" s="35" t="s">
-        <v>27</v>
-      </c>
-      <c r="E72" s="7">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="73" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D73" s="37" t="s">
-        <v>30</v>
-      </c>
-      <c r="E73" s="7">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="74" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D74" s="37" t="s">
-        <v>48</v>
-      </c>
-      <c r="E74" s="7">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="75" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D75" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="E75" s="7">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="76" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="E76" s="7">
-        <f>SUM(E68:E75)</f>
-        <v>309</v>
-      </c>
-    </row>
-    <row r="77" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="E77" s="7">
-        <f>E76*1460000</f>
-        <v>451140000</v>
-      </c>
-    </row>
-    <row r="78" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D78" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="E78" s="7">
-        <f>735527814+25496237</f>
-        <v>761024051</v>
-      </c>
-    </row>
-    <row r="79" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="E79" s="7">
-        <f>E78-E77</f>
-        <v>309884051</v>
-      </c>
+      <c r="B66" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C66" s="8">
+        <v>32</v>
+      </c>
+      <c r="D66" s="10"/>
+      <c r="E66" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F66" s="38" t="s">
+        <v>114</v>
+      </c>
+      <c r="G66" s="38"/>
+      <c r="H66" s="38"/>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E67" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F67" s="38"/>
     </row>
   </sheetData>
   <pageMargins left="0.43" right="0.12" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
cetak spatu dan topi bn dp1n9
</commit_message>
<xml_diff>
--- a/RENCANA BON VOYAGE.xlsx
+++ b/RENCANA BON VOYAGE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mapan\progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F115F88-1979-4F6E-BEE8-9D60A8D62ED6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC621786-E8BD-4404-A436-DFC4252E19FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="123">
   <si>
     <t>NO</t>
   </si>
@@ -374,6 +374,27 @@
   </si>
   <si>
     <t>RISKY</t>
+  </si>
+  <si>
+    <t>67 ORANG</t>
+  </si>
+  <si>
+    <t>14 ORANG</t>
+  </si>
+  <si>
+    <t>SUNARTO</t>
+  </si>
+  <si>
+    <t>JAMALUDIN</t>
+  </si>
+  <si>
+    <t>ABIDIN</t>
+  </si>
+  <si>
+    <t>27 AGUSTUS</t>
+  </si>
+  <si>
+    <t>20 AGUSTUS</t>
   </si>
 </sst>
 </file>
@@ -615,7 +636,7 @@
     <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -959,13 +980,13 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:O58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="H58" sqref="A1:H58"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="F57" sqref="F57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.28515625" style="40" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.140625" style="7" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.85546875" style="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.5703125" style="40" bestFit="1" customWidth="1"/>
@@ -980,7 +1001,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="41" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
@@ -1009,7 +1030,7 @@
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A2" s="8">
+      <c r="A2" s="38">
         <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
@@ -1038,7 +1059,7 @@
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A3" s="8"/>
+      <c r="A3" s="38"/>
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
       <c r="D3" s="38"/>
@@ -1057,7 +1078,7 @@
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A4" s="8"/>
+      <c r="A4" s="38"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
       <c r="D4" s="38"/>
@@ -1067,7 +1088,7 @@
       <c r="H4" s="8"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A5" s="8">
+      <c r="A5" s="38">
         <v>2</v>
       </c>
       <c r="B5" s="8" t="s">
@@ -1096,7 +1117,7 @@
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A6" s="8"/>
+      <c r="A6" s="38"/>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
       <c r="D6" s="38"/>
@@ -1112,7 +1133,7 @@
       <c r="H6" s="8"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A7" s="8"/>
+      <c r="A7" s="38"/>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
       <c r="D7" s="38"/>
@@ -1122,7 +1143,7 @@
       <c r="H7" s="8"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A8" s="8">
+      <c r="A8" s="38">
         <v>3</v>
       </c>
       <c r="B8" s="8" t="s">
@@ -1151,7 +1172,7 @@
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A9" s="8"/>
+      <c r="A9" s="38"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
       <c r="D9" s="38"/>
@@ -1167,7 +1188,7 @@
       <c r="H9" s="9"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A10" s="8"/>
+      <c r="A10" s="38"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
       <c r="D10" s="38"/>
@@ -1177,7 +1198,7 @@
       <c r="H10" s="9"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A11" s="8">
+      <c r="A11" s="38">
         <v>4</v>
       </c>
       <c r="B11" s="8" t="s">
@@ -1206,7 +1227,7 @@
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A12" s="8"/>
+      <c r="A12" s="38"/>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
       <c r="D12" s="38"/>
@@ -1222,7 +1243,7 @@
       <c r="H12" s="9"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A13" s="8"/>
+      <c r="A13" s="38"/>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
       <c r="D13" s="38"/>
@@ -1232,7 +1253,7 @@
       <c r="H13" s="9"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A14" s="37">
+      <c r="A14" s="42">
         <v>5</v>
       </c>
       <c r="B14" s="37" t="s">
@@ -1261,7 +1282,7 @@
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A15" s="37"/>
+      <c r="A15" s="42"/>
       <c r="B15" s="37"/>
       <c r="C15" s="37"/>
       <c r="D15" s="42"/>
@@ -1277,7 +1298,7 @@
       <c r="H15" s="8"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A16" s="37"/>
+      <c r="A16" s="42"/>
       <c r="B16" s="37"/>
       <c r="C16" s="37"/>
       <c r="D16" s="42"/>
@@ -1286,8 +1307,8 @@
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A17" s="37">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="42">
         <v>6</v>
       </c>
       <c r="B17" s="37" t="s">
@@ -1315,8 +1336,8 @@
         <v>102</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A18" s="37"/>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="42"/>
       <c r="B18" s="37"/>
       <c r="C18" s="37"/>
       <c r="D18" s="42"/>
@@ -1331,8 +1352,8 @@
       </c>
       <c r="H18" s="8"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A19" s="37"/>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="42"/>
       <c r="B19" s="37"/>
       <c r="C19" s="37"/>
       <c r="D19" s="42"/>
@@ -1341,8 +1362,8 @@
       <c r="G19" s="8"/>
       <c r="H19" s="8"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A20" s="37">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="42">
         <v>7</v>
       </c>
       <c r="B20" s="37" t="s">
@@ -1370,8 +1391,8 @@
         <v>102</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A21" s="37"/>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="42"/>
       <c r="B21" s="37"/>
       <c r="C21" s="37"/>
       <c r="D21" s="42"/>
@@ -1389,8 +1410,8 @@
         <v>102</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A22" s="37"/>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="42"/>
       <c r="B22" s="37"/>
       <c r="C22" s="37"/>
       <c r="D22" s="42"/>
@@ -1399,8 +1420,8 @@
       <c r="G22" s="8"/>
       <c r="H22" s="8"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A23" s="37">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="42">
         <v>8</v>
       </c>
       <c r="B23" s="37" t="s">
@@ -1428,15 +1449,15 @@
         <v>102</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A24" s="37"/>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="42"/>
       <c r="B24" s="37"/>
       <c r="C24" s="37"/>
       <c r="D24" s="42"/>
-      <c r="E24" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="F24" s="8" t="s">
+      <c r="E24" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="F24" s="35" t="s">
         <v>87</v>
       </c>
       <c r="G24" s="8">
@@ -1444,8 +1465,8 @@
       </c>
       <c r="H24" s="8"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A25" s="37"/>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="42"/>
       <c r="B25" s="37"/>
       <c r="C25" s="37"/>
       <c r="D25" s="42"/>
@@ -1454,8 +1475,8 @@
       <c r="G25" s="8"/>
       <c r="H25" s="8"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A26" s="37">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="42">
         <v>9</v>
       </c>
       <c r="B26" s="37" t="s">
@@ -1483,15 +1504,15 @@
         <v>44287</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A27" s="37"/>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="42"/>
       <c r="B27" s="37"/>
       <c r="C27" s="37"/>
       <c r="D27" s="42"/>
-      <c r="E27" s="32" t="s">
-        <v>8</v>
-      </c>
-      <c r="F27" s="32" t="s">
+      <c r="E27" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="F27" s="35" t="s">
         <v>87</v>
       </c>
       <c r="G27" s="32" t="s">
@@ -1499,8 +1520,8 @@
       </c>
       <c r="H27" s="33"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A28" s="8"/>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" s="38"/>
       <c r="B28" s="8"/>
       <c r="C28" s="8"/>
       <c r="D28" s="38"/>
@@ -1509,8 +1530,8 @@
       <c r="G28" s="8"/>
       <c r="H28" s="8"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A29" s="35">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" s="43">
         <v>10</v>
       </c>
       <c r="B29" s="35" t="s">
@@ -1538,8 +1559,8 @@
         <v>114</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A30" s="8"/>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" s="38"/>
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>
       <c r="D30" s="38"/>
@@ -1554,8 +1575,8 @@
       </c>
       <c r="H30" s="8"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A31" s="10"/>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" s="38"/>
       <c r="B31" s="10"/>
       <c r="C31" s="10"/>
       <c r="D31" s="38"/>
@@ -1563,9 +1584,10 @@
       <c r="F31" s="10"/>
       <c r="G31" s="10"/>
       <c r="H31" s="10"/>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A32" s="35">
+      <c r="I31" s="7"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" s="43">
         <v>11</v>
       </c>
       <c r="B32" s="35" t="s">
@@ -1589,15 +1611,12 @@
       <c r="H32" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="I32" s="45" t="s">
+      <c r="I32" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="J32" s="12"/>
-      <c r="K32" s="12"/>
-      <c r="L32" s="12"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33" s="32"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A33" s="45"/>
       <c r="B33" s="8"/>
       <c r="C33" s="8"/>
       <c r="D33" s="38"/>
@@ -1611,9 +1630,10 @@
         <v>101</v>
       </c>
       <c r="H33" s="8"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34" s="8"/>
+      <c r="I33" s="7"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A34" s="38"/>
       <c r="B34" s="8"/>
       <c r="C34" s="8"/>
       <c r="D34" s="38"/>
@@ -1621,9 +1641,10 @@
       <c r="F34" s="8"/>
       <c r="G34" s="8"/>
       <c r="H34" s="8"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A35" s="8">
+      <c r="I34" s="7"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A35" s="38">
         <v>12</v>
       </c>
       <c r="B35" s="8" t="s">
@@ -1647,9 +1668,10 @@
       <c r="H35" s="9">
         <v>44444</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A36" s="8"/>
+      <c r="I35" s="7"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A36" s="38"/>
       <c r="B36" s="8"/>
       <c r="C36" s="8"/>
       <c r="D36" s="38"/>
@@ -1663,9 +1685,10 @@
         <v>81331414130</v>
       </c>
       <c r="H36" s="8"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A37" s="8"/>
+      <c r="I36" s="7"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A37" s="38"/>
       <c r="B37" s="8"/>
       <c r="C37" s="8"/>
       <c r="D37" s="38"/>
@@ -1673,9 +1696,10 @@
       <c r="F37" s="8"/>
       <c r="G37" s="8"/>
       <c r="H37" s="8"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A38" s="8">
+      <c r="I37" s="7"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A38" s="38">
         <v>13</v>
       </c>
       <c r="B38" s="8" t="s">
@@ -1699,9 +1723,10 @@
       <c r="H38" s="9">
         <v>44444</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A39" s="8"/>
+      <c r="I38" s="7"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A39" s="38"/>
       <c r="B39" s="8"/>
       <c r="C39" s="8"/>
       <c r="D39" s="38"/>
@@ -1716,8 +1741,8 @@
       </c>
       <c r="H39" s="8"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A40" s="8"/>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A40" s="38"/>
       <c r="B40" s="8"/>
       <c r="C40" s="8"/>
       <c r="D40" s="38"/>
@@ -1726,8 +1751,8 @@
       <c r="G40" s="8"/>
       <c r="H40" s="8"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A41" s="8">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A41" s="38">
         <v>14</v>
       </c>
       <c r="B41" s="8" t="s">
@@ -1752,22 +1777,24 @@
         <v>104</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A42" s="8"/>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A42" s="38"/>
       <c r="B42" s="8"/>
       <c r="C42" s="8"/>
       <c r="D42" s="38"/>
       <c r="E42" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="F42" s="10"/>
+      <c r="F42" s="9">
+        <v>44614</v>
+      </c>
       <c r="G42" s="8">
         <v>85732094240</v>
       </c>
       <c r="H42" s="10"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A43" s="10"/>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A43" s="38"/>
       <c r="B43" s="10"/>
       <c r="C43" s="10"/>
       <c r="D43" s="38"/>
@@ -1776,7 +1803,7 @@
       <c r="G43" s="10"/>
       <c r="H43" s="10"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="38">
         <v>15</v>
       </c>
@@ -1802,8 +1829,8 @@
         <v>108</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A45" s="10"/>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A45" s="38"/>
       <c r="B45" s="10"/>
       <c r="C45" s="8"/>
       <c r="D45" s="38"/>
@@ -1818,7 +1845,7 @@
       </c>
       <c r="H45" s="38"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="38"/>
       <c r="B46" s="10"/>
       <c r="C46" s="8"/>
@@ -1828,7 +1855,7 @@
       <c r="G46" s="38"/>
       <c r="H46" s="38"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="38">
         <v>16</v>
       </c>
@@ -1854,8 +1881,8 @@
         <v>111</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A48" s="10"/>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A48" s="38"/>
       <c r="B48" s="10"/>
       <c r="C48" s="8"/>
       <c r="D48" s="38"/>
@@ -1881,7 +1908,7 @@
       <c r="H49" s="38"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A50" s="10">
+      <c r="A50" s="38">
         <v>17</v>
       </c>
       <c r="B50" s="10" t="s">
@@ -1890,12 +1917,18 @@
       <c r="C50" s="8">
         <v>17</v>
       </c>
-      <c r="D50" s="38"/>
+      <c r="D50" s="38" t="s">
+        <v>116</v>
+      </c>
       <c r="E50" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="F50" s="39"/>
-      <c r="G50" s="38"/>
+      <c r="F50" s="39" t="s">
+        <v>121</v>
+      </c>
+      <c r="G50" s="38" t="s">
+        <v>120</v>
+      </c>
       <c r="H50" s="38"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
@@ -1907,11 +1940,13 @@
         <v>8</v>
       </c>
       <c r="F51" s="38"/>
-      <c r="G51" s="38"/>
+      <c r="G51" s="38">
+        <v>81284663664</v>
+      </c>
       <c r="H51" s="38"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A52" s="10"/>
+      <c r="A52" s="38"/>
       <c r="B52" s="10"/>
       <c r="C52" s="8"/>
       <c r="D52" s="38"/>
@@ -1930,16 +1965,22 @@
       <c r="C53" s="8">
         <v>17</v>
       </c>
-      <c r="D53" s="38"/>
+      <c r="D53" s="38" t="s">
+        <v>49</v>
+      </c>
       <c r="E53" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="F53" s="38"/>
-      <c r="G53" s="38"/>
+      <c r="F53" s="39" t="s">
+        <v>121</v>
+      </c>
+      <c r="G53" s="38" t="s">
+        <v>119</v>
+      </c>
       <c r="H53" s="38"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A54" s="10"/>
+      <c r="A54" s="38"/>
       <c r="B54" s="10"/>
       <c r="C54" s="8"/>
       <c r="D54" s="38"/>
@@ -1947,7 +1988,9 @@
         <v>8</v>
       </c>
       <c r="F54" s="39"/>
-      <c r="G54" s="38"/>
+      <c r="G54" s="38">
+        <v>85740346667</v>
+      </c>
       <c r="H54" s="38"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
@@ -1961,7 +2004,7 @@
       <c r="H55" s="38"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A56" s="10">
+      <c r="A56" s="38">
         <v>19</v>
       </c>
       <c r="B56" s="10" t="s">
@@ -1970,12 +2013,18 @@
       <c r="C56" s="8">
         <v>33</v>
       </c>
-      <c r="D56" s="38"/>
+      <c r="D56" s="38" t="s">
+        <v>117</v>
+      </c>
       <c r="E56" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="F56" s="39"/>
-      <c r="G56" s="38"/>
+      <c r="F56" s="39" t="s">
+        <v>122</v>
+      </c>
+      <c r="G56" s="38" t="s">
+        <v>118</v>
+      </c>
       <c r="H56" s="38"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
@@ -1987,11 +2036,13 @@
         <v>8</v>
       </c>
       <c r="F57" s="38"/>
-      <c r="G57" s="38"/>
+      <c r="G57" s="38">
+        <v>81331430509</v>
+      </c>
       <c r="H57" s="38"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A58" s="10"/>
+      <c r="A58" s="38"/>
       <c r="B58" s="10"/>
       <c r="C58" s="8"/>
       <c r="D58" s="38"/>

</xml_diff>

<commit_message>
update rencana bon voyage
</commit_message>
<xml_diff>
--- a/RENCANA BON VOYAGE.xlsx
+++ b/RENCANA BON VOYAGE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mapan\progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73D39C76-08DC-4B4B-9893-E0427729819B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3152103C-EA12-4ECE-AC14-96EDDED56B03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,14 +19,14 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$55</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$40</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="128">
   <si>
     <t>NO</t>
   </si>
@@ -388,9 +388,6 @@
     <t>JAMALUDIN</t>
   </si>
   <si>
-    <t>ABIDIN</t>
-  </si>
-  <si>
     <t>27 AGUSTUS</t>
   </si>
   <si>
@@ -406,19 +403,13 @@
     <t>YOSEP</t>
   </si>
   <si>
-    <t>Sum</t>
-  </si>
-  <si>
-    <t>Average</t>
-  </si>
-  <si>
-    <t>Running Total</t>
-  </si>
-  <si>
-    <t>Count</t>
-  </si>
-  <si>
     <t>ZAINUL</t>
+  </si>
+  <si>
+    <t>17 ORANG</t>
+  </si>
+  <si>
+    <t>15 ORANG</t>
   </si>
 </sst>
 </file>
@@ -476,7 +467,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -536,11 +527,91 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -663,10 +734,46 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1008,10 +1115,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:O73"/>
+  <dimension ref="A1:O71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="111" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="111" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="F65" sqref="F65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1097,7 +1204,7 @@
         <v>8</v>
       </c>
       <c r="F3" s="35" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G3" s="8">
         <v>81228196787</v>
@@ -1155,7 +1262,7 @@
         <v>8</v>
       </c>
       <c r="F6" s="35" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G6" s="8">
         <v>81225736355</v>
@@ -1174,7 +1281,7 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="38">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>6</v>
@@ -1190,7 +1297,7 @@
       </c>
       <c r="F8" s="37"/>
       <c r="G8" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H8" s="9"/>
     </row>
@@ -1223,7 +1330,7 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="38">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>15</v>
@@ -1265,7 +1372,7 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="38">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>20</v>
@@ -1300,7 +1407,7 @@
       <c r="E15" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="F15" s="47">
+      <c r="F15" s="46">
         <v>44501</v>
       </c>
       <c r="G15" s="8">
@@ -1320,7 +1427,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="38">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>22</v>
@@ -1375,7 +1482,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="38">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B20" s="8" t="s">
         <v>20</v>
@@ -1389,9 +1496,11 @@
       <c r="E20" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="F20" s="37"/>
+      <c r="F20" s="37" t="s">
+        <v>120</v>
+      </c>
       <c r="G20" s="8" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="H20" s="9"/>
     </row>
@@ -1403,7 +1512,7 @@
       <c r="E21" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="F21" s="47"/>
+      <c r="F21" s="46"/>
       <c r="G21" s="8">
         <v>81284663664</v>
       </c>
@@ -1421,7 +1530,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="38">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>22</v>
@@ -1435,8 +1544,12 @@
       <c r="E23" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="F23" s="37"/>
-      <c r="G23" s="8"/>
+      <c r="F23" s="37" t="s">
+        <v>120</v>
+      </c>
+      <c r="G23" s="38" t="s">
+        <v>119</v>
+      </c>
       <c r="H23" s="9"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
@@ -1448,7 +1561,9 @@
         <v>8</v>
       </c>
       <c r="F24" s="34"/>
-      <c r="G24" s="8"/>
+      <c r="G24" s="38">
+        <v>85740346667</v>
+      </c>
       <c r="H24" s="9"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
@@ -1473,7 +1588,7 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="42">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B27" s="37" t="s">
         <v>26</v>
@@ -1528,7 +1643,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="42">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B30" s="37" t="s">
         <v>26</v>
@@ -1537,7 +1652,7 @@
         <v>31</v>
       </c>
       <c r="D30" s="42" t="s">
-        <v>53</v>
+        <v>110</v>
       </c>
       <c r="E30" s="35" t="s">
         <v>7</v>
@@ -1582,87 +1697,81 @@
       <c r="H32" s="8"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A33" s="42">
-        <v>7</v>
-      </c>
-      <c r="B33" s="37" t="s">
-        <v>24</v>
-      </c>
-      <c r="C33" s="37">
-        <v>25</v>
-      </c>
-      <c r="D33" s="42" t="s">
-        <v>48</v>
-      </c>
-      <c r="E33" s="35" t="s">
-        <v>7</v>
-      </c>
-      <c r="F33" s="36">
-        <v>44237</v>
-      </c>
-      <c r="G33" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="H33" s="9">
-        <v>44501</v>
-      </c>
-      <c r="I33" s="40" t="s">
-        <v>102</v>
+      <c r="A33" s="38">
+        <v>11</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C33" s="8">
+        <v>32</v>
+      </c>
+      <c r="D33" s="38" t="s">
+        <v>110</v>
+      </c>
+      <c r="E33" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F33" s="38" t="s">
+        <v>109</v>
+      </c>
+      <c r="G33" s="38" t="s">
+        <v>115</v>
+      </c>
+      <c r="H33" s="38" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A34" s="42"/>
-      <c r="B34" s="37"/>
-      <c r="C34" s="37"/>
-      <c r="D34" s="42"/>
+      <c r="A34" s="38"/>
+      <c r="B34" s="10"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="38"/>
       <c r="E34" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="F34" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="G34" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="H34" s="8"/>
-      <c r="I34" s="40" t="s">
-        <v>102</v>
-      </c>
+      <c r="F34" s="39">
+        <v>44520</v>
+      </c>
+      <c r="G34" s="38">
+        <v>81333524165</v>
+      </c>
+      <c r="H34" s="38"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A35" s="42"/>
-      <c r="B35" s="37"/>
-      <c r="C35" s="37"/>
-      <c r="D35" s="42"/>
+      <c r="A35" s="38"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="38"/>
       <c r="E35" s="8"/>
-      <c r="F35" s="8"/>
-      <c r="G35" s="8"/>
-      <c r="H35" s="8"/>
+      <c r="F35" s="38"/>
+      <c r="G35" s="38"/>
+      <c r="H35" s="38"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="42">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B36" s="37" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="C36" s="37">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="D36" s="42" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="E36" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="F36" s="35" t="s">
-        <v>86</v>
+      <c r="F36" s="36">
+        <v>44237</v>
       </c>
       <c r="G36" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="H36" s="8" t="s">
-        <v>66</v>
+        <v>94</v>
+      </c>
+      <c r="H36" s="9">
+        <v>44501</v>
       </c>
       <c r="I36" s="40" t="s">
         <v>102</v>
@@ -1673,16 +1782,19 @@
       <c r="B37" s="37"/>
       <c r="C37" s="37"/>
       <c r="D37" s="42"/>
-      <c r="E37" s="35" t="s">
-        <v>8</v>
-      </c>
-      <c r="F37" s="35" t="s">
-        <v>87</v>
-      </c>
-      <c r="G37" s="8">
-        <v>81231558203</v>
+      <c r="E37" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F37" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="G37" s="8" t="s">
+        <v>95</v>
       </c>
       <c r="H37" s="8"/>
+      <c r="I37" s="40" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="42"/>
@@ -1695,216 +1807,204 @@
       <c r="H38" s="8"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A39" s="42">
-        <v>9</v>
-      </c>
-      <c r="B39" s="37" t="s">
-        <v>38</v>
-      </c>
-      <c r="C39" s="37">
-        <v>27</v>
-      </c>
-      <c r="D39" s="42" t="s">
-        <v>67</v>
+      <c r="A39" s="38">
+        <v>13</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C39" s="8">
+        <v>26</v>
+      </c>
+      <c r="D39" s="38" t="s">
+        <v>48</v>
       </c>
       <c r="E39" s="35" t="s">
         <v>7</v>
       </c>
       <c r="F39" s="35" t="s">
-        <v>88</v>
-      </c>
-      <c r="G39" s="32" t="s">
-        <v>98</v>
-      </c>
-      <c r="H39" s="33">
-        <v>44409</v>
-      </c>
-      <c r="I39" s="44">
-        <v>44287</v>
+        <v>105</v>
+      </c>
+      <c r="G39" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="H39" s="9" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A40" s="42"/>
-      <c r="B40" s="37"/>
-      <c r="C40" s="37"/>
-      <c r="D40" s="42"/>
-      <c r="E40" s="35" t="s">
-        <v>8</v>
-      </c>
-      <c r="F40" s="35" t="s">
-        <v>87</v>
-      </c>
-      <c r="G40" s="32" t="s">
-        <v>99</v>
-      </c>
-      <c r="H40" s="33"/>
+      <c r="A40" s="38"/>
+      <c r="B40" s="8"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="38"/>
+      <c r="E40" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F40" s="9">
+        <v>44614</v>
+      </c>
+      <c r="G40" s="8">
+        <v>85732094240</v>
+      </c>
+      <c r="H40" s="10"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="38"/>
-      <c r="B41" s="8"/>
-      <c r="C41" s="8"/>
+      <c r="B41" s="10"/>
+      <c r="C41" s="10"/>
       <c r="D41" s="38"/>
-      <c r="E41" s="8"/>
-      <c r="F41" s="8"/>
-      <c r="G41" s="8"/>
-      <c r="H41" s="8"/>
+      <c r="E41" s="10"/>
+      <c r="F41" s="10"/>
+      <c r="G41" s="10"/>
+      <c r="H41" s="10"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A42" s="43">
-        <v>10</v>
-      </c>
-      <c r="B42" s="35" t="s">
-        <v>39</v>
-      </c>
-      <c r="C42" s="35">
-        <v>38</v>
-      </c>
-      <c r="D42" s="43" t="s">
-        <v>50</v>
+      <c r="A42" s="42">
+        <v>14</v>
+      </c>
+      <c r="B42" s="37" t="s">
+        <v>36</v>
+      </c>
+      <c r="C42" s="37">
+        <v>32</v>
+      </c>
+      <c r="D42" s="42" t="s">
+        <v>25</v>
       </c>
       <c r="E42" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="F42" s="36">
-        <v>44253</v>
+      <c r="F42" s="35" t="s">
+        <v>86</v>
       </c>
       <c r="G42" s="8" t="s">
-        <v>96</v>
+        <v>65</v>
       </c>
       <c r="H42" s="8" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="I42" s="40" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A43" s="38"/>
-      <c r="B43" s="8"/>
-      <c r="C43" s="8"/>
-      <c r="D43" s="38"/>
+      <c r="A43" s="42"/>
+      <c r="B43" s="37"/>
+      <c r="C43" s="37"/>
+      <c r="D43" s="42"/>
       <c r="E43" s="35" t="s">
         <v>8</v>
       </c>
       <c r="F43" s="35" t="s">
-        <v>84</v>
-      </c>
-      <c r="G43" s="8" t="s">
-        <v>97</v>
+        <v>87</v>
+      </c>
+      <c r="G43" s="8">
+        <v>81231558203</v>
       </c>
       <c r="H43" s="8"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A44" s="38"/>
-      <c r="B44" s="10"/>
-      <c r="C44" s="10"/>
-      <c r="D44" s="38"/>
-      <c r="E44" s="10"/>
-      <c r="F44" s="10"/>
-      <c r="G44" s="10"/>
-      <c r="H44" s="10"/>
-      <c r="I44" s="7"/>
+      <c r="A44" s="42"/>
+      <c r="B44" s="37"/>
+      <c r="C44" s="37"/>
+      <c r="D44" s="42"/>
+      <c r="E44" s="8"/>
+      <c r="F44" s="8"/>
+      <c r="G44" s="8"/>
+      <c r="H44" s="8"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A45" s="43">
-        <v>11</v>
-      </c>
-      <c r="B45" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="C45" s="35">
-        <v>38</v>
-      </c>
-      <c r="D45" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="E45" s="35" t="s">
-        <v>7</v>
-      </c>
-      <c r="F45" s="36">
-        <v>44253</v>
-      </c>
-      <c r="G45" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="H45" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="I45" s="7" t="s">
-        <v>114</v>
-      </c>
+      <c r="A45" s="38">
+        <v>15</v>
+      </c>
+      <c r="B45" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C45" s="8">
+        <v>33</v>
+      </c>
+      <c r="D45" s="38" t="s">
+        <v>117</v>
+      </c>
+      <c r="E45" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F45" s="39" t="s">
+        <v>121</v>
+      </c>
+      <c r="G45" s="38" t="s">
+        <v>118</v>
+      </c>
+      <c r="H45" s="38"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A46" s="45"/>
-      <c r="B46" s="8"/>
+      <c r="A46" s="38"/>
+      <c r="B46" s="10"/>
       <c r="C46" s="8"/>
       <c r="D46" s="38"/>
-      <c r="E46" s="35" t="s">
-        <v>8</v>
-      </c>
-      <c r="F46" s="35" t="s">
-        <v>89</v>
-      </c>
-      <c r="G46" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="H46" s="8"/>
-      <c r="I46" s="7"/>
+      <c r="E46" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F46" s="38"/>
+      <c r="G46" s="38">
+        <v>81331430509</v>
+      </c>
+      <c r="H46" s="38"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A47" s="38"/>
-      <c r="B47" s="8"/>
-      <c r="C47" s="8"/>
-      <c r="D47" s="38"/>
+      <c r="A47" s="42"/>
+      <c r="B47" s="37"/>
+      <c r="C47" s="37"/>
+      <c r="D47" s="42"/>
       <c r="E47" s="8"/>
       <c r="F47" s="8"/>
       <c r="G47" s="8"/>
       <c r="H47" s="8"/>
-      <c r="I47" s="7"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A48" s="38">
-        <v>12</v>
-      </c>
-      <c r="B48" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C48" s="8">
-        <v>39</v>
-      </c>
-      <c r="D48" s="38" t="s">
-        <v>25</v>
+      <c r="A48" s="42">
+        <v>16</v>
+      </c>
+      <c r="B48" s="37" t="s">
+        <v>38</v>
+      </c>
+      <c r="C48" s="37">
+        <v>27</v>
+      </c>
+      <c r="D48" s="42" t="s">
+        <v>67</v>
       </c>
       <c r="E48" s="35" t="s">
         <v>7</v>
       </c>
       <c r="F48" s="35" t="s">
-        <v>82</v>
-      </c>
-      <c r="G48" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="H48" s="9">
-        <v>44444</v>
-      </c>
-      <c r="I48" s="7"/>
+        <v>88</v>
+      </c>
+      <c r="G48" s="32" t="s">
+        <v>98</v>
+      </c>
+      <c r="H48" s="33">
+        <v>44409</v>
+      </c>
+      <c r="I48" s="44">
+        <v>44287</v>
+      </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A49" s="38"/>
-      <c r="B49" s="8"/>
-      <c r="C49" s="8"/>
-      <c r="D49" s="38"/>
-      <c r="E49" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="F49" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="G49" s="8">
-        <v>81331414130</v>
-      </c>
-      <c r="H49" s="8"/>
-      <c r="I49" s="7"/>
+      <c r="A49" s="42"/>
+      <c r="B49" s="37"/>
+      <c r="C49" s="37"/>
+      <c r="D49" s="42"/>
+      <c r="E49" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="F49" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="G49" s="32" t="s">
+        <v>99</v>
+      </c>
+      <c r="H49" s="33"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" s="38"/>
@@ -1915,85 +2015,86 @@
       <c r="F50" s="8"/>
       <c r="G50" s="8"/>
       <c r="H50" s="8"/>
-      <c r="I50" s="7"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="38">
-        <v>13</v>
-      </c>
-      <c r="B51" s="8" t="s">
-        <v>41</v>
+        <v>17</v>
+      </c>
+      <c r="B51" s="10" t="s">
+        <v>38</v>
       </c>
       <c r="C51" s="8">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="D51" s="38" t="s">
-        <v>69</v>
-      </c>
-      <c r="E51" s="35" t="s">
-        <v>7</v>
-      </c>
-      <c r="F51" s="35" t="s">
-        <v>82</v>
-      </c>
-      <c r="G51" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="H51" s="9">
-        <v>44444</v>
-      </c>
-      <c r="I51" s="7"/>
+        <v>112</v>
+      </c>
+      <c r="E51" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F51" s="38" t="s">
+        <v>106</v>
+      </c>
+      <c r="G51" s="38" t="s">
+        <v>107</v>
+      </c>
+      <c r="H51" s="38" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" s="38"/>
-      <c r="B52" s="8"/>
+      <c r="B52" s="10"/>
       <c r="C52" s="8"/>
       <c r="D52" s="38"/>
       <c r="E52" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="F52" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="G52" s="8">
-        <v>81252283477</v>
-      </c>
-      <c r="H52" s="8"/>
+      <c r="F52" s="39">
+        <v>44501</v>
+      </c>
+      <c r="G52" s="38">
+        <v>85649115380</v>
+      </c>
+      <c r="H52" s="38"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" s="38"/>
-      <c r="B53" s="8"/>
+      <c r="B53" s="10"/>
       <c r="C53" s="8"/>
       <c r="D53" s="38"/>
       <c r="E53" s="8"/>
-      <c r="F53" s="8"/>
-      <c r="G53" s="8"/>
-      <c r="H53" s="8"/>
+      <c r="F53" s="38"/>
+      <c r="G53" s="38"/>
+      <c r="H53" s="38"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A54" s="38">
-        <v>14</v>
-      </c>
-      <c r="B54" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C54" s="8">
-        <v>26</v>
-      </c>
-      <c r="D54" s="38" t="s">
-        <v>48</v>
+      <c r="A54" s="43">
+        <v>18</v>
+      </c>
+      <c r="B54" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="C54" s="35">
+        <v>38</v>
+      </c>
+      <c r="D54" s="43" t="s">
+        <v>50</v>
       </c>
       <c r="E54" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="F54" s="35" t="s">
-        <v>105</v>
+      <c r="F54" s="36">
+        <v>44253</v>
       </c>
       <c r="G54" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="H54" s="9" t="s">
-        <v>104</v>
+        <v>96</v>
+      </c>
+      <c r="H54" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="I54" s="40" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
@@ -2001,16 +2102,16 @@
       <c r="B55" s="8"/>
       <c r="C55" s="8"/>
       <c r="D55" s="38"/>
-      <c r="E55" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="F55" s="9">
-        <v>44614</v>
-      </c>
-      <c r="G55" s="8">
-        <v>85732094240</v>
-      </c>
-      <c r="H55" s="10"/>
+      <c r="E55" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="F55" s="35" t="s">
+        <v>84</v>
+      </c>
+      <c r="G55" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="H55" s="8"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" s="38"/>
@@ -2021,276 +2122,261 @@
       <c r="F56" s="10"/>
       <c r="G56" s="10"/>
       <c r="H56" s="10"/>
+      <c r="I56" s="7"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A57" s="38">
-        <v>15</v>
-      </c>
-      <c r="B57" s="10" t="s">
+      <c r="A57" s="43">
+        <v>19</v>
+      </c>
+      <c r="B57" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="C57" s="35">
         <v>38</v>
       </c>
-      <c r="C57" s="8">
-        <v>28</v>
-      </c>
-      <c r="D57" s="38" t="s">
-        <v>112</v>
-      </c>
-      <c r="E57" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F57" s="38" t="s">
-        <v>106</v>
-      </c>
-      <c r="G57" s="38" t="s">
-        <v>107</v>
-      </c>
-      <c r="H57" s="38" t="s">
-        <v>108</v>
+      <c r="D57" s="43" t="s">
+        <v>48</v>
+      </c>
+      <c r="E57" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="F57" s="36">
+        <v>44253</v>
+      </c>
+      <c r="G57" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="H57" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="I57" s="7" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A58" s="38"/>
-      <c r="B58" s="10"/>
+      <c r="A58" s="45"/>
+      <c r="B58" s="8"/>
       <c r="C58" s="8"/>
       <c r="D58" s="38"/>
-      <c r="E58" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="F58" s="39">
-        <v>44501</v>
-      </c>
-      <c r="G58" s="38">
-        <v>85649115380</v>
-      </c>
-      <c r="H58" s="38"/>
+      <c r="E58" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="F58" s="35" t="s">
+        <v>89</v>
+      </c>
+      <c r="G58" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="H58" s="8"/>
+      <c r="I58" s="7"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" s="38"/>
-      <c r="B59" s="10"/>
+      <c r="B59" s="8"/>
       <c r="C59" s="8"/>
       <c r="D59" s="38"/>
       <c r="E59" s="8"/>
-      <c r="F59" s="38"/>
-      <c r="G59" s="38"/>
-      <c r="H59" s="38"/>
+      <c r="F59" s="8"/>
+      <c r="G59" s="8"/>
+      <c r="H59" s="8"/>
+      <c r="I59" s="7"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" s="38">
-        <v>16</v>
-      </c>
-      <c r="B60" s="10" t="s">
-        <v>26</v>
+        <v>20</v>
+      </c>
+      <c r="B60" s="8" t="s">
+        <v>39</v>
       </c>
       <c r="C60" s="8">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="D60" s="38" t="s">
-        <v>110</v>
-      </c>
-      <c r="E60" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F60" s="38" t="s">
-        <v>109</v>
-      </c>
-      <c r="G60" s="38" t="s">
-        <v>115</v>
-      </c>
-      <c r="H60" s="38" t="s">
-        <v>111</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="E60" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="F60" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="G60" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="H60" s="9">
+        <v>44444</v>
+      </c>
+      <c r="I60" s="7"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" s="38"/>
-      <c r="B61" s="10"/>
+      <c r="B61" s="8"/>
       <c r="C61" s="8"/>
       <c r="D61" s="38"/>
       <c r="E61" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="F61" s="39">
-        <v>44520</v>
-      </c>
-      <c r="G61" s="38">
-        <v>81333524165</v>
-      </c>
-      <c r="H61" s="38"/>
+      <c r="F61" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="G61" s="8">
+        <v>81331414130</v>
+      </c>
+      <c r="H61" s="8"/>
+      <c r="I61" s="7"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" s="38"/>
-      <c r="B62" s="10"/>
+      <c r="B62" s="8"/>
       <c r="C62" s="8"/>
       <c r="D62" s="38"/>
       <c r="E62" s="8"/>
-      <c r="F62" s="38"/>
-      <c r="G62" s="38"/>
-      <c r="H62" s="38"/>
+      <c r="F62" s="8"/>
+      <c r="G62" s="8"/>
+      <c r="H62" s="8"/>
+      <c r="I62" s="7"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" s="38">
-        <v>17</v>
-      </c>
-      <c r="B63" s="10" t="s">
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c r="B63" s="8" t="s">
+        <v>41</v>
       </c>
       <c r="C63" s="8">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="D63" s="38" t="s">
-        <v>116</v>
-      </c>
-      <c r="E63" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F63" s="39" t="s">
-        <v>121</v>
-      </c>
-      <c r="G63" s="38" t="s">
-        <v>120</v>
-      </c>
-      <c r="H63" s="38"/>
+        <v>69</v>
+      </c>
+      <c r="E63" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="F63" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="G63" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="H63" s="9">
+        <v>44444</v>
+      </c>
+      <c r="I63" s="7"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" s="38"/>
-      <c r="B64" s="10"/>
+      <c r="B64" s="8"/>
       <c r="C64" s="8"/>
       <c r="D64" s="38"/>
       <c r="E64" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="F64" s="38"/>
-      <c r="G64" s="38">
-        <v>81284663664</v>
-      </c>
-      <c r="H64" s="38"/>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F64" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="G64" s="8">
+        <v>81252283477</v>
+      </c>
+      <c r="H64" s="8"/>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" s="38"/>
-      <c r="B65" s="10"/>
+      <c r="B65" s="8"/>
       <c r="C65" s="8"/>
       <c r="D65" s="38"/>
       <c r="E65" s="8"/>
-      <c r="F65" s="39"/>
-      <c r="G65" s="38"/>
-      <c r="H65" s="38"/>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A66" s="38">
-        <v>18</v>
-      </c>
-      <c r="B66" s="10" t="s">
+      <c r="F65" s="8"/>
+      <c r="G65" s="8"/>
+      <c r="H65" s="8"/>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A66" s="47">
         <v>22</v>
       </c>
-      <c r="C66" s="8">
-        <v>17</v>
-      </c>
-      <c r="D66" s="38" t="s">
-        <v>49</v>
-      </c>
-      <c r="E66" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F66" s="39" t="s">
-        <v>121</v>
-      </c>
-      <c r="G66" s="38" t="s">
-        <v>119</v>
-      </c>
-      <c r="H66" s="38"/>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A67" s="38"/>
-      <c r="B67" s="10"/>
-      <c r="C67" s="8"/>
-      <c r="D67" s="38"/>
-      <c r="E67" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="F67" s="39"/>
-      <c r="G67" s="38">
-        <v>85740346667</v>
-      </c>
-      <c r="H67" s="38"/>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A68" s="38"/>
-      <c r="B68" s="10"/>
-      <c r="C68" s="8"/>
-      <c r="D68" s="38"/>
-      <c r="E68" s="8"/>
-      <c r="F68" s="38"/>
-      <c r="G68" s="38"/>
-      <c r="H68" s="38"/>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A69" s="38">
-        <v>19</v>
-      </c>
-      <c r="B69" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="C69" s="8">
-        <v>33</v>
-      </c>
-      <c r="D69" s="38" t="s">
-        <v>117</v>
-      </c>
-      <c r="E69" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F69" s="39" t="s">
+      <c r="B66" s="48" t="s">
+        <v>39</v>
+      </c>
+      <c r="C66" s="49">
+        <v>40</v>
+      </c>
+      <c r="D66" s="50" t="s">
+        <v>127</v>
+      </c>
+      <c r="E66" s="48" t="s">
+        <v>7</v>
+      </c>
+      <c r="F66" s="48"/>
+      <c r="G66" s="50" t="s">
         <v>122</v>
       </c>
-      <c r="G69" s="38" t="s">
-        <v>118</v>
-      </c>
-      <c r="H69" s="38"/>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A70" s="38"/>
-      <c r="B70" s="10"/>
-      <c r="C70" s="8"/>
-      <c r="D70" s="38"/>
-      <c r="E70" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="F70" s="38"/>
-      <c r="G70" s="38">
-        <v>81331430509</v>
-      </c>
-      <c r="H70" s="38"/>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A71" s="38"/>
-      <c r="B71" s="10"/>
-      <c r="C71" s="8"/>
-      <c r="D71" s="38"/>
-      <c r="E71" s="8"/>
-      <c r="F71" s="39"/>
-      <c r="G71" s="38"/>
-      <c r="H71" s="38"/>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B72" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C72" s="46">
+      <c r="H66" s="51"/>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A67" s="52"/>
+      <c r="B67" s="53"/>
+      <c r="C67" s="53"/>
+      <c r="D67" s="54"/>
+      <c r="E67" s="53" t="s">
+        <v>8</v>
+      </c>
+      <c r="F67" s="53"/>
+      <c r="G67" s="54">
+        <v>81359524067</v>
+      </c>
+      <c r="H67" s="55"/>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A68" s="56"/>
+      <c r="B68" s="57"/>
+      <c r="C68" s="57"/>
+      <c r="D68" s="58"/>
+      <c r="E68" s="57"/>
+      <c r="F68" s="57"/>
+      <c r="G68" s="57"/>
+      <c r="H68" s="59"/>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A69" s="50">
+        <v>23</v>
+      </c>
+      <c r="B69" s="49" t="s">
+        <v>41</v>
+      </c>
+      <c r="C69" s="49">
         <v>40</v>
       </c>
-      <c r="E72" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="G72" s="40" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="E73" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G73" s="40">
-        <v>81359524067</v>
-      </c>
+      <c r="D69" s="50" t="s">
+        <v>126</v>
+      </c>
+      <c r="E69" s="60" t="s">
+        <v>7</v>
+      </c>
+      <c r="F69" s="60"/>
+      <c r="G69" s="49"/>
+      <c r="H69" s="61"/>
+      <c r="I69" s="7"/>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A70" s="54"/>
+      <c r="B70" s="62"/>
+      <c r="C70" s="62"/>
+      <c r="D70" s="54"/>
+      <c r="E70" s="62" t="s">
+        <v>8</v>
+      </c>
+      <c r="F70" s="62"/>
+      <c r="G70" s="62"/>
+      <c r="H70" s="62"/>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A71" s="58"/>
+      <c r="B71" s="63"/>
+      <c r="C71" s="63"/>
+      <c r="D71" s="58"/>
+      <c r="E71" s="63"/>
+      <c r="F71" s="63"/>
+      <c r="G71" s="63"/>
+      <c r="H71" s="63"/>
     </row>
   </sheetData>
   <pageMargins left="0.43" right="0.12" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update bonvoyage dan dp3t27
</commit_message>
<xml_diff>
--- a/RENCANA BON VOYAGE.xlsx
+++ b/RENCANA BON VOYAGE.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24430"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mapan\progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E409A4A-C40A-4FAD-A1B1-11D0AF670A3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{312D42A5-2E56-48D5-B88E-140073D895AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="138">
   <si>
     <t>NO</t>
   </si>
@@ -421,6 +421,24 @@
   </si>
   <si>
     <t>06 OKT</t>
+  </si>
+  <si>
+    <t>ILHAM</t>
+  </si>
+  <si>
+    <t>26 OKT</t>
+  </si>
+  <si>
+    <t>10 JUN 22</t>
+  </si>
+  <si>
+    <t>081216290006</t>
+  </si>
+  <si>
+    <t>10 MEI 22</t>
+  </si>
+  <si>
+    <t>14 OKT</t>
   </si>
 </sst>
 </file>
@@ -567,7 +585,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="119">
+  <cellXfs count="120">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -619,9 +637,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="15" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -794,9 +809,6 @@
     <xf numFmtId="16" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="15" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
@@ -910,6 +922,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1528,8 +1549,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:J65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1539,55 +1560,55 @@
     <col min="3" max="3" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17" style="2" customWidth="1"/>
     <col min="5" max="5" width="18.42578125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" style="34" customWidth="1"/>
-    <col min="7" max="7" width="21.5703125" style="71" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" style="33" customWidth="1"/>
+    <col min="7" max="7" width="21.5703125" style="70" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.42578125" style="57" customWidth="1"/>
-    <col min="10" max="10" width="14" style="29" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" style="56" customWidth="1"/>
+    <col min="10" max="10" width="14" style="28" bestFit="1" customWidth="1"/>
     <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="106" t="s">
+      <c r="A1" s="104" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="106" t="s">
+      <c r="B1" s="104" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="106" t="s">
+      <c r="C1" s="104" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="112" t="s">
+      <c r="D1" s="110" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="112"/>
-      <c r="F1" s="110" t="s">
+      <c r="E1" s="110"/>
+      <c r="F1" s="108" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="108" t="s">
+      <c r="G1" s="106" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="106" t="s">
+      <c r="H1" s="104" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="106" t="s">
+      <c r="I1" s="104" t="s">
         <v>56</v>
       </c>
-      <c r="J1" s="106"/>
+      <c r="J1" s="104"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="107"/>
-      <c r="B2" s="107"/>
-      <c r="C2" s="107"/>
+      <c r="A2" s="105"/>
+      <c r="B2" s="105"/>
+      <c r="C2" s="105"/>
       <c r="D2" s="17" t="s">
         <v>6</v>
       </c>
       <c r="E2" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="111"/>
-      <c r="G2" s="109"/>
-      <c r="H2" s="107"/>
+      <c r="F2" s="109"/>
+      <c r="G2" s="107"/>
+      <c r="H2" s="105"/>
       <c r="I2" s="17" t="s">
         <v>6</v>
       </c>
@@ -1599,119 +1620,119 @@
       <c r="A3" s="5">
         <v>1</v>
       </c>
-      <c r="B3" s="102" t="s">
+      <c r="B3" s="100" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="4">
         <v>10</v>
       </c>
-      <c r="D3" s="77" t="s">
+      <c r="D3" s="76" t="s">
         <v>107</v>
       </c>
-      <c r="E3" s="99" t="s">
+      <c r="E3" s="97" t="s">
         <v>95</v>
       </c>
-      <c r="F3" s="81" t="s">
+      <c r="F3" s="79" t="s">
         <v>52</v>
       </c>
-      <c r="G3" s="67" t="s">
+      <c r="G3" s="66" t="s">
         <v>50</v>
       </c>
       <c r="H3" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="I3" s="72" t="s">
+      <c r="I3" s="71" t="s">
         <v>98</v>
       </c>
-      <c r="J3" s="27"/>
+      <c r="J3" s="26"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="7"/>
-      <c r="B4" s="28"/>
+      <c r="B4" s="27"/>
       <c r="C4" s="11"/>
       <c r="D4" s="20"/>
       <c r="E4" s="20"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="65">
+      <c r="F4" s="29"/>
+      <c r="G4" s="64">
         <v>81331434743</v>
       </c>
       <c r="H4" s="7"/>
-      <c r="I4" s="28"/>
-      <c r="J4" s="25"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="24"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="9"/>
-      <c r="B5" s="53"/>
+      <c r="B5" s="52"/>
       <c r="C5" s="12"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="66"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="65"/>
       <c r="H5" s="9"/>
-      <c r="I5" s="53"/>
-      <c r="J5" s="26"/>
+      <c r="I5" s="52"/>
+      <c r="J5" s="25"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="5">
         <v>2</v>
       </c>
-      <c r="B6" s="102" t="s">
+      <c r="B6" s="100" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="4">
         <v>10</v>
       </c>
-      <c r="D6" s="77" t="s">
+      <c r="D6" s="76" t="s">
         <v>107</v>
       </c>
-      <c r="E6" s="99" t="s">
+      <c r="E6" s="97" t="s">
         <v>95</v>
       </c>
-      <c r="F6" s="81" t="s">
+      <c r="F6" s="79" t="s">
         <v>52</v>
       </c>
-      <c r="G6" s="67" t="s">
+      <c r="G6" s="66" t="s">
         <v>99</v>
       </c>
       <c r="H6" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="I6" s="72" t="s">
+      <c r="I6" s="71" t="s">
         <v>98</v>
       </c>
-      <c r="J6" s="27"/>
+      <c r="J6" s="26"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="7"/>
-      <c r="B7" s="28"/>
+      <c r="B7" s="27"/>
       <c r="C7" s="11"/>
       <c r="D7" s="20"/>
       <c r="E7" s="20"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="73" t="s">
+      <c r="F7" s="29"/>
+      <c r="G7" s="72" t="s">
         <v>100</v>
       </c>
       <c r="H7" s="7"/>
-      <c r="I7" s="28"/>
-      <c r="J7" s="25"/>
+      <c r="I7" s="27"/>
+      <c r="J7" s="24"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="9"/>
-      <c r="B8" s="53"/>
+      <c r="B8" s="52"/>
       <c r="C8" s="12"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="31"/>
-      <c r="G8" s="66"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="65"/>
       <c r="H8" s="9"/>
-      <c r="I8" s="53"/>
-      <c r="J8" s="26"/>
+      <c r="I8" s="52"/>
+      <c r="J8" s="25"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="5">
         <v>3</v>
       </c>
-      <c r="B9" s="102" t="s">
+      <c r="B9" s="100" t="s">
         <v>10</v>
       </c>
       <c r="C9" s="4">
@@ -1720,54 +1741,54 @@
       <c r="D9" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="E9" s="75" t="s">
+      <c r="E9" s="74" t="s">
         <v>129</v>
       </c>
-      <c r="F9" s="98">
+      <c r="F9" s="96">
         <v>44520</v>
       </c>
-      <c r="G9" s="67" t="s">
+      <c r="G9" s="66" t="s">
         <v>21</v>
       </c>
       <c r="H9" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="I9" s="54" t="s">
+      <c r="I9" s="53" t="s">
         <v>53</v>
       </c>
-      <c r="J9" s="27"/>
+      <c r="J9" s="26"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="7"/>
-      <c r="B10" s="28"/>
+      <c r="B10" s="27"/>
       <c r="C10" s="11"/>
       <c r="D10" s="7"/>
-      <c r="E10" s="37"/>
-      <c r="F10" s="35"/>
-      <c r="G10" s="65">
+      <c r="E10" s="36"/>
+      <c r="F10" s="34"/>
+      <c r="G10" s="64">
         <v>81232989078</v>
       </c>
       <c r="H10" s="7"/>
-      <c r="I10" s="28"/>
-      <c r="J10" s="25"/>
+      <c r="I10" s="27"/>
+      <c r="J10" s="24"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="9"/>
-      <c r="B11" s="53"/>
+      <c r="B11" s="52"/>
       <c r="C11" s="12"/>
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="66"/>
+      <c r="F11" s="37"/>
+      <c r="G11" s="65"/>
       <c r="H11" s="9"/>
-      <c r="I11" s="53"/>
-      <c r="J11" s="26"/>
+      <c r="I11" s="52"/>
+      <c r="J11" s="25"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="5">
         <v>4</v>
       </c>
-      <c r="B12" s="102" t="s">
+      <c r="B12" s="100" t="s">
         <v>11</v>
       </c>
       <c r="C12" s="4">
@@ -1776,168 +1797,168 @@
       <c r="D12" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="E12" s="75" t="s">
+      <c r="E12" s="74" t="s">
         <v>129</v>
       </c>
-      <c r="F12" s="98">
+      <c r="F12" s="96">
         <v>44520</v>
       </c>
-      <c r="G12" s="67" t="s">
+      <c r="G12" s="66" t="s">
         <v>22</v>
       </c>
       <c r="H12" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="I12" s="54" t="s">
+      <c r="I12" s="53" t="s">
         <v>53</v>
       </c>
-      <c r="J12" s="27"/>
+      <c r="J12" s="26"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="7"/>
-      <c r="B13" s="28"/>
+      <c r="B13" s="27"/>
       <c r="C13" s="11"/>
       <c r="D13" s="7"/>
-      <c r="E13" s="37"/>
-      <c r="F13" s="35"/>
-      <c r="G13" s="65">
+      <c r="E13" s="36"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="64">
         <v>81231807990</v>
       </c>
       <c r="H13" s="7"/>
-      <c r="I13" s="28"/>
-      <c r="J13" s="25"/>
+      <c r="I13" s="27"/>
+      <c r="J13" s="24"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="9"/>
-      <c r="B14" s="53"/>
+      <c r="B14" s="52"/>
       <c r="C14" s="12"/>
       <c r="D14" s="9"/>
       <c r="E14" s="9"/>
-      <c r="F14" s="38"/>
-      <c r="G14" s="66"/>
+      <c r="F14" s="37"/>
+      <c r="G14" s="65"/>
       <c r="H14" s="9"/>
-      <c r="I14" s="53"/>
-      <c r="J14" s="26"/>
+      <c r="I14" s="52"/>
+      <c r="J14" s="25"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="5">
         <v>5</v>
       </c>
-      <c r="B15" s="102" t="s">
+      <c r="B15" s="100" t="s">
         <v>10</v>
       </c>
       <c r="C15" s="4">
         <v>17</v>
       </c>
-      <c r="D15" s="78" t="s">
+      <c r="D15" s="77" t="s">
         <v>108</v>
       </c>
-      <c r="E15" s="99" t="s">
+      <c r="E15" s="97" t="s">
         <v>130</v>
       </c>
-      <c r="F15" s="90" t="s">
+      <c r="F15" s="88" t="s">
         <v>65</v>
       </c>
-      <c r="G15" s="67" t="s">
+      <c r="G15" s="66" t="s">
         <v>51</v>
       </c>
       <c r="H15" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="I15" s="55">
+      <c r="I15" s="54">
         <v>44449</v>
       </c>
-      <c r="J15" s="27"/>
+      <c r="J15" s="26"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="7"/>
-      <c r="B16" s="28"/>
+      <c r="B16" s="27"/>
       <c r="C16" s="11"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="37">
+      <c r="D16" s="36"/>
+      <c r="E16" s="36">
         <v>1</v>
       </c>
-      <c r="F16" s="35"/>
-      <c r="G16" s="65">
+      <c r="F16" s="34"/>
+      <c r="G16" s="64">
         <v>81284663664</v>
       </c>
       <c r="H16" s="7"/>
-      <c r="I16" s="28"/>
-      <c r="J16" s="25"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="24"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="9"/>
-      <c r="B17" s="53"/>
+      <c r="B17" s="52"/>
       <c r="C17" s="12"/>
-      <c r="D17" s="22"/>
-      <c r="E17" s="22"/>
-      <c r="F17" s="38"/>
-      <c r="G17" s="66"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="37"/>
+      <c r="G17" s="65"/>
       <c r="H17" s="9"/>
-      <c r="I17" s="53"/>
-      <c r="J17" s="26"/>
+      <c r="I17" s="52"/>
+      <c r="J17" s="25"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="5">
         <v>6</v>
       </c>
-      <c r="B18" s="102" t="s">
+      <c r="B18" s="100" t="s">
         <v>11</v>
       </c>
       <c r="C18" s="4">
         <v>17</v>
       </c>
-      <c r="D18" s="78" t="s">
+      <c r="D18" s="77" t="s">
         <v>108</v>
       </c>
-      <c r="E18" s="99" t="s">
+      <c r="E18" s="97" t="s">
         <v>130</v>
       </c>
-      <c r="F18" s="90" t="s">
+      <c r="F18" s="88" t="s">
         <v>65</v>
       </c>
-      <c r="G18" s="67" t="s">
+      <c r="G18" s="66" t="s">
         <v>47</v>
       </c>
       <c r="H18" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="I18" s="55">
+      <c r="I18" s="54">
         <v>44449</v>
       </c>
-      <c r="J18" s="27"/>
+      <c r="J18" s="26"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="7"/>
-      <c r="B19" s="28"/>
+      <c r="B19" s="27"/>
       <c r="C19" s="11"/>
-      <c r="D19" s="37"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="35"/>
-      <c r="G19" s="65">
+      <c r="D19" s="36"/>
+      <c r="E19" s="36"/>
+      <c r="F19" s="34"/>
+      <c r="G19" s="64">
         <v>85740346667</v>
       </c>
       <c r="H19" s="7"/>
-      <c r="I19" s="28"/>
-      <c r="J19" s="25"/>
+      <c r="I19" s="27"/>
+      <c r="J19" s="24"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="9"/>
-      <c r="B20" s="53"/>
+      <c r="B20" s="52"/>
       <c r="C20" s="12"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="38"/>
-      <c r="G20" s="66"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="37"/>
+      <c r="G20" s="65"/>
       <c r="H20" s="9"/>
-      <c r="I20" s="53"/>
-      <c r="J20" s="26"/>
+      <c r="I20" s="52"/>
+      <c r="J20" s="25"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="5">
         <v>7</v>
       </c>
-      <c r="B21" s="103" t="s">
+      <c r="B21" s="101" t="s">
         <v>13</v>
       </c>
       <c r="C21" s="10">
@@ -1946,54 +1967,54 @@
       <c r="D21" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="E21" s="77" t="s">
+      <c r="E21" s="76" t="s">
         <v>131</v>
       </c>
-      <c r="F21" s="95">
+      <c r="F21" s="93">
         <v>44501</v>
       </c>
-      <c r="G21" s="67" t="s">
+      <c r="G21" s="66" t="s">
         <v>23</v>
       </c>
-      <c r="H21" s="24" t="s">
+      <c r="H21" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="I21" s="54" t="s">
+      <c r="I21" s="53" t="s">
         <v>53</v>
       </c>
-      <c r="J21" s="27"/>
+      <c r="J21" s="26"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="7"/>
-      <c r="B22" s="104"/>
+      <c r="B22" s="102"/>
       <c r="C22" s="15"/>
       <c r="D22" s="7"/>
-      <c r="E22" s="45"/>
-      <c r="F22" s="30"/>
-      <c r="G22" s="65">
+      <c r="E22" s="44"/>
+      <c r="F22" s="29"/>
+      <c r="G22" s="64">
         <v>6587623904</v>
       </c>
       <c r="H22" s="20"/>
-      <c r="I22" s="28"/>
-      <c r="J22" s="25"/>
+      <c r="I22" s="27"/>
+      <c r="J22" s="24"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="9"/>
-      <c r="B23" s="105"/>
+      <c r="B23" s="103"/>
       <c r="C23" s="16"/>
       <c r="D23" s="9"/>
       <c r="E23" s="9"/>
-      <c r="F23" s="31"/>
-      <c r="G23" s="66"/>
-      <c r="H23" s="22"/>
-      <c r="I23" s="53"/>
-      <c r="J23" s="26"/>
+      <c r="F23" s="30"/>
+      <c r="G23" s="65"/>
+      <c r="H23" s="21"/>
+      <c r="I23" s="52"/>
+      <c r="J23" s="25"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="5">
         <v>8</v>
       </c>
-      <c r="B24" s="102" t="s">
+      <c r="B24" s="100" t="s">
         <v>13</v>
       </c>
       <c r="C24" s="4">
@@ -2002,166 +2023,168 @@
       <c r="D24" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="E24" s="23">
+      <c r="E24" s="22">
         <v>44520</v>
       </c>
-      <c r="F24" s="82" t="s">
+      <c r="F24" s="80" t="s">
         <v>44</v>
       </c>
-      <c r="G24" s="68" t="s">
+      <c r="G24" s="67" t="s">
         <v>45</v>
       </c>
       <c r="H24" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="I24" s="55">
+      <c r="I24" s="54">
         <v>44440</v>
       </c>
-      <c r="J24" s="27"/>
+      <c r="J24" s="26"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="7"/>
-      <c r="B25" s="28"/>
+      <c r="B25" s="27"/>
       <c r="C25" s="11"/>
-      <c r="D25" s="45"/>
-      <c r="E25" s="45"/>
-      <c r="F25" s="33"/>
-      <c r="G25" s="69">
+      <c r="D25" s="44"/>
+      <c r="E25" s="44"/>
+      <c r="F25" s="32"/>
+      <c r="G25" s="68">
         <v>81333524165</v>
       </c>
       <c r="H25" s="7"/>
-      <c r="I25" s="28"/>
-      <c r="J25" s="25"/>
+      <c r="I25" s="27"/>
+      <c r="J25" s="24"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="9"/>
-      <c r="B26" s="53"/>
+      <c r="B26" s="52"/>
       <c r="C26" s="12"/>
       <c r="D26" s="9"/>
       <c r="E26" s="9"/>
-      <c r="F26" s="46"/>
-      <c r="G26" s="70"/>
+      <c r="F26" s="45"/>
+      <c r="G26" s="69"/>
       <c r="H26" s="9"/>
-      <c r="I26" s="53"/>
-      <c r="J26" s="26"/>
+      <c r="I26" s="52"/>
+      <c r="J26" s="25"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="5">
         <v>9</v>
       </c>
-      <c r="B27" s="102" t="s">
+      <c r="B27" s="100" t="s">
         <v>13</v>
       </c>
       <c r="C27" s="4">
         <v>33</v>
       </c>
-      <c r="D27" s="78" t="s">
+      <c r="D27" s="77" t="s">
         <v>108</v>
       </c>
-      <c r="E27" s="45">
+      <c r="E27" s="44">
         <v>44247</v>
       </c>
-      <c r="F27" s="91" t="s">
+      <c r="F27" s="89" t="s">
         <v>103</v>
       </c>
-      <c r="G27" s="69" t="s">
+      <c r="G27" s="68" t="s">
         <v>101</v>
       </c>
       <c r="H27" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="I27" s="28"/>
-      <c r="J27" s="25"/>
+      <c r="I27" s="119" t="s">
+        <v>137</v>
+      </c>
+      <c r="J27" s="24"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="7"/>
-      <c r="B28" s="28"/>
+      <c r="B28" s="27"/>
       <c r="C28" s="11"/>
       <c r="D28" s="7"/>
       <c r="E28" s="7"/>
-      <c r="F28" s="33"/>
-      <c r="G28" s="69">
+      <c r="F28" s="32"/>
+      <c r="G28" s="68">
         <v>81235748714</v>
       </c>
       <c r="H28" s="7"/>
-      <c r="I28" s="28"/>
-      <c r="J28" s="25"/>
+      <c r="I28" s="27"/>
+      <c r="J28" s="24"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="9"/>
-      <c r="B29" s="28"/>
+      <c r="B29" s="27"/>
       <c r="C29" s="11"/>
       <c r="D29" s="7"/>
       <c r="E29" s="7"/>
-      <c r="F29" s="33"/>
-      <c r="G29" s="69"/>
+      <c r="F29" s="32"/>
+      <c r="G29" s="68"/>
       <c r="H29" s="7"/>
-      <c r="I29" s="28"/>
-      <c r="J29" s="25"/>
+      <c r="I29" s="27"/>
+      <c r="J29" s="24"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="5">
         <v>10</v>
       </c>
-      <c r="B30" s="103" t="s">
+      <c r="B30" s="101" t="s">
         <v>12</v>
       </c>
       <c r="C30" s="10">
         <v>25</v>
       </c>
-      <c r="D30" s="44">
+      <c r="D30" s="43">
         <v>44237</v>
       </c>
       <c r="E30" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="F30" s="95">
+      <c r="F30" s="93">
         <v>44501</v>
       </c>
-      <c r="G30" s="67" t="s">
+      <c r="G30" s="66" t="s">
         <v>35</v>
       </c>
-      <c r="H30" s="24" t="s">
+      <c r="H30" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="I30" s="54" t="s">
+      <c r="I30" s="53" t="s">
         <v>53</v>
       </c>
-      <c r="J30" s="54" t="s">
+      <c r="J30" s="53" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="7"/>
-      <c r="B31" s="104"/>
+      <c r="B31" s="102"/>
       <c r="C31" s="15"/>
       <c r="D31" s="7"/>
       <c r="E31" s="7"/>
-      <c r="F31" s="30"/>
-      <c r="G31" s="65">
+      <c r="F31" s="29"/>
+      <c r="G31" s="64">
         <v>82143316439</v>
       </c>
       <c r="H31" s="20"/>
-      <c r="I31" s="28"/>
-      <c r="J31" s="25"/>
+      <c r="I31" s="27"/>
+      <c r="J31" s="24"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="9"/>
-      <c r="B32" s="105"/>
+      <c r="B32" s="103"/>
       <c r="C32" s="16"/>
       <c r="D32" s="9"/>
       <c r="E32" s="9"/>
-      <c r="F32" s="31"/>
-      <c r="G32" s="66"/>
-      <c r="H32" s="22"/>
-      <c r="I32" s="53"/>
-      <c r="J32" s="26"/>
+      <c r="F32" s="30"/>
+      <c r="G32" s="65"/>
+      <c r="H32" s="21"/>
+      <c r="I32" s="52"/>
+      <c r="J32" s="25"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="5">
         <v>11</v>
       </c>
-      <c r="B33" s="102" t="s">
+      <c r="B33" s="100" t="s">
         <v>12</v>
       </c>
       <c r="C33" s="4">
@@ -2170,96 +2193,108 @@
       <c r="D33" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="E33" s="47">
+      <c r="E33" s="46">
         <v>44614</v>
       </c>
-      <c r="F33" s="90" t="s">
+      <c r="F33" s="88" t="s">
         <v>61</v>
       </c>
-      <c r="G33" s="67" t="s">
+      <c r="G33" s="66" t="s">
         <v>60</v>
       </c>
       <c r="H33" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="I33" s="55">
+      <c r="I33" s="54">
         <v>44440</v>
       </c>
-      <c r="J33" s="27"/>
+      <c r="J33" s="26"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="7"/>
-      <c r="B34" s="28"/>
+      <c r="B34" s="27"/>
       <c r="C34" s="11"/>
       <c r="D34" s="7"/>
-      <c r="E34" s="48"/>
-      <c r="F34" s="30"/>
-      <c r="G34" s="65">
+      <c r="E34" s="47"/>
+      <c r="F34" s="29"/>
+      <c r="G34" s="64">
         <v>85732094240</v>
       </c>
       <c r="H34" s="7"/>
-      <c r="I34" s="28"/>
-      <c r="J34" s="25"/>
+      <c r="I34" s="27"/>
+      <c r="J34" s="24"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="9"/>
-      <c r="B35" s="53"/>
+      <c r="B35" s="52"/>
       <c r="C35" s="8"/>
       <c r="D35" s="9"/>
       <c r="E35" s="9"/>
-      <c r="F35" s="31"/>
-      <c r="G35" s="66"/>
+      <c r="F35" s="30"/>
+      <c r="G35" s="65"/>
       <c r="H35" s="9"/>
-      <c r="I35" s="53"/>
-      <c r="J35" s="26"/>
+      <c r="I35" s="52"/>
+      <c r="J35" s="25"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="5">
         <v>12</v>
       </c>
-      <c r="B36" s="102" t="s">
+      <c r="B36" s="100" t="s">
         <v>12</v>
       </c>
       <c r="C36" s="4">
         <v>27</v>
       </c>
-      <c r="D36" s="24"/>
-      <c r="E36" s="21"/>
-      <c r="F36" s="36"/>
-      <c r="G36" s="67"/>
-      <c r="H36" s="5"/>
-      <c r="I36" s="79"/>
-      <c r="J36" s="27"/>
+      <c r="D36" s="23" t="s">
+        <v>133</v>
+      </c>
+      <c r="E36" s="97" t="s">
+        <v>136</v>
+      </c>
+      <c r="F36" s="118" t="s">
+        <v>134</v>
+      </c>
+      <c r="G36" s="66" t="s">
+        <v>132</v>
+      </c>
+      <c r="H36" s="117" t="s">
+        <v>89</v>
+      </c>
+      <c r="I36" s="78"/>
+      <c r="J36" s="26"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="7"/>
-      <c r="B37" s="28"/>
+      <c r="B37" s="27"/>
       <c r="C37" s="11"/>
       <c r="D37" s="7"/>
-      <c r="E37" s="48"/>
-      <c r="F37" s="30"/>
-      <c r="G37" s="65"/>
+      <c r="E37" s="47"/>
+      <c r="F37" s="29"/>
+      <c r="G37" s="72" t="s">
+        <v>135</v>
+      </c>
       <c r="H37" s="7"/>
-      <c r="I37" s="28"/>
-      <c r="J37" s="25"/>
+      <c r="I37" s="27"/>
+      <c r="J37" s="24"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="9"/>
-      <c r="B38" s="53"/>
+      <c r="B38" s="52"/>
       <c r="C38" s="8"/>
       <c r="D38" s="9"/>
       <c r="E38" s="9"/>
-      <c r="F38" s="31"/>
-      <c r="G38" s="66"/>
+      <c r="F38" s="30"/>
+      <c r="G38" s="65"/>
       <c r="H38" s="9"/>
-      <c r="I38" s="53"/>
-      <c r="J38" s="26"/>
+      <c r="I38" s="52"/>
+      <c r="J38" s="25"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="5">
         <v>13</v>
       </c>
-      <c r="B39" s="102" t="s">
+      <c r="B39" s="100" t="s">
         <v>14</v>
       </c>
       <c r="C39" s="4">
@@ -2268,54 +2303,54 @@
       <c r="D39" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="E39" s="77" t="s">
+      <c r="E39" s="76" t="s">
         <v>131</v>
       </c>
-      <c r="F39" s="96">
+      <c r="F39" s="94">
         <v>44510</v>
       </c>
-      <c r="G39" s="68" t="s">
+      <c r="G39" s="67" t="s">
         <v>46</v>
       </c>
       <c r="H39" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="I39" s="55">
+      <c r="I39" s="54">
         <v>44449</v>
       </c>
-      <c r="J39" s="27"/>
+      <c r="J39" s="26"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" s="7"/>
-      <c r="B40" s="28"/>
+      <c r="B40" s="27"/>
       <c r="C40" s="11"/>
-      <c r="D40" s="45"/>
-      <c r="E40" s="45"/>
-      <c r="F40" s="33"/>
-      <c r="G40" s="69">
+      <c r="D40" s="44"/>
+      <c r="E40" s="44"/>
+      <c r="F40" s="32"/>
+      <c r="G40" s="68">
         <v>81331430509</v>
       </c>
       <c r="H40" s="7"/>
-      <c r="I40" s="28"/>
-      <c r="J40" s="25"/>
+      <c r="I40" s="27"/>
+      <c r="J40" s="24"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="9"/>
-      <c r="B41" s="53"/>
+      <c r="B41" s="52"/>
       <c r="C41" s="12"/>
       <c r="D41" s="9"/>
       <c r="E41" s="9"/>
-      <c r="F41" s="46"/>
-      <c r="G41" s="70"/>
+      <c r="F41" s="45"/>
+      <c r="G41" s="69"/>
       <c r="H41" s="9"/>
-      <c r="I41" s="53"/>
-      <c r="J41" s="26"/>
+      <c r="I41" s="52"/>
+      <c r="J41" s="25"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" s="5">
         <v>14</v>
       </c>
-      <c r="B42" s="102" t="s">
+      <c r="B42" s="100" t="s">
         <v>15</v>
       </c>
       <c r="C42" s="4">
@@ -2324,160 +2359,160 @@
       <c r="D42" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="E42" s="76" t="s">
+      <c r="E42" s="75" t="s">
         <v>95</v>
       </c>
-      <c r="F42" s="83" t="s">
+      <c r="F42" s="81" t="s">
         <v>42</v>
       </c>
-      <c r="G42" s="68" t="s">
+      <c r="G42" s="67" t="s">
         <v>41</v>
       </c>
       <c r="H42" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="I42" s="55">
+      <c r="I42" s="54">
         <v>44440</v>
       </c>
-      <c r="J42" s="27"/>
+      <c r="J42" s="26"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" s="7"/>
-      <c r="B43" s="28"/>
+      <c r="B43" s="27"/>
       <c r="C43" s="11"/>
-      <c r="D43" s="45"/>
-      <c r="E43" s="45"/>
-      <c r="F43" s="33"/>
-      <c r="G43" s="69">
+      <c r="D43" s="44"/>
+      <c r="E43" s="44"/>
+      <c r="F43" s="32"/>
+      <c r="G43" s="68">
         <v>85649115380</v>
       </c>
       <c r="H43" s="7"/>
-      <c r="I43" s="28"/>
-      <c r="J43" s="25"/>
+      <c r="I43" s="27"/>
+      <c r="J43" s="24"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" s="9"/>
-      <c r="B44" s="53"/>
+      <c r="B44" s="52"/>
       <c r="C44" s="12"/>
       <c r="D44" s="9"/>
       <c r="E44" s="9"/>
-      <c r="F44" s="46"/>
-      <c r="G44" s="70"/>
+      <c r="F44" s="45"/>
+      <c r="G44" s="69"/>
       <c r="H44" s="9"/>
-      <c r="I44" s="53"/>
-      <c r="J44" s="26"/>
+      <c r="I44" s="52"/>
+      <c r="J44" s="25"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" s="5">
         <v>15</v>
       </c>
-      <c r="B45" s="102" t="s">
+      <c r="B45" s="100" t="s">
         <v>16</v>
       </c>
       <c r="C45" s="4">
         <v>40</v>
       </c>
-      <c r="D45" s="44">
+      <c r="D45" s="43">
         <v>44453</v>
       </c>
-      <c r="E45" s="76" t="s">
+      <c r="E45" s="75" t="s">
         <v>95</v>
       </c>
-      <c r="F45" s="83" t="s">
+      <c r="F45" s="81" t="s">
         <v>42</v>
       </c>
-      <c r="G45" s="68" t="s">
+      <c r="G45" s="67" t="s">
         <v>48</v>
       </c>
       <c r="H45" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="I45" s="72" t="s">
+      <c r="I45" s="71" t="s">
         <v>98</v>
       </c>
-      <c r="J45" s="27"/>
+      <c r="J45" s="26"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" s="7"/>
-      <c r="B46" s="28"/>
+      <c r="B46" s="27"/>
       <c r="C46" s="11"/>
-      <c r="D46" s="45"/>
-      <c r="E46" s="45"/>
-      <c r="F46" s="33"/>
-      <c r="G46" s="69">
+      <c r="D46" s="44"/>
+      <c r="E46" s="44"/>
+      <c r="F46" s="32"/>
+      <c r="G46" s="68">
         <v>81359524067</v>
       </c>
       <c r="H46" s="7"/>
-      <c r="I46" s="28"/>
-      <c r="J46" s="25"/>
+      <c r="I46" s="27"/>
+      <c r="J46" s="24"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" s="9"/>
-      <c r="B47" s="53"/>
+      <c r="B47" s="52"/>
       <c r="C47" s="12"/>
       <c r="D47" s="9"/>
       <c r="E47" s="9"/>
-      <c r="F47" s="46"/>
-      <c r="G47" s="70"/>
+      <c r="F47" s="45"/>
+      <c r="G47" s="69"/>
       <c r="H47" s="9"/>
-      <c r="I47" s="53"/>
-      <c r="J47" s="26"/>
+      <c r="I47" s="52"/>
+      <c r="J47" s="25"/>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" s="5">
         <v>16</v>
       </c>
-      <c r="B48" s="102" t="s">
+      <c r="B48" s="100" t="s">
         <v>18</v>
       </c>
       <c r="C48" s="4">
         <v>40</v>
       </c>
-      <c r="D48" s="44">
+      <c r="D48" s="43">
         <v>44453</v>
       </c>
-      <c r="E48" s="76" t="s">
+      <c r="E48" s="75" t="s">
         <v>95</v>
       </c>
-      <c r="F48" s="83" t="s">
+      <c r="F48" s="81" t="s">
         <v>42</v>
       </c>
-      <c r="G48" s="68" t="s">
+      <c r="G48" s="67" t="s">
         <v>25</v>
       </c>
       <c r="H48" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="I48" s="72" t="s">
+      <c r="I48" s="71" t="s">
         <v>98</v>
       </c>
-      <c r="J48" s="27"/>
+      <c r="J48" s="26"/>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" s="7"/>
-      <c r="B49" s="28"/>
+      <c r="B49" s="27"/>
       <c r="C49" s="11"/>
-      <c r="D49" s="45"/>
-      <c r="E49" s="45"/>
-      <c r="F49" s="33"/>
-      <c r="G49" s="69">
+      <c r="D49" s="44"/>
+      <c r="E49" s="44"/>
+      <c r="F49" s="32"/>
+      <c r="G49" s="68">
         <v>82319844744</v>
       </c>
       <c r="H49" s="7"/>
-      <c r="I49" s="28"/>
-      <c r="J49" s="25"/>
+      <c r="I49" s="27"/>
+      <c r="J49" s="24"/>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" s="9"/>
-      <c r="B50" s="53"/>
+      <c r="B50" s="52"/>
       <c r="C50" s="12"/>
       <c r="D50" s="9"/>
       <c r="E50" s="9"/>
-      <c r="F50" s="46"/>
-      <c r="G50" s="70"/>
+      <c r="F50" s="45"/>
+      <c r="G50" s="69"/>
       <c r="H50" s="9"/>
-      <c r="I50" s="53"/>
-      <c r="J50" s="26"/>
+      <c r="I50" s="52"/>
+      <c r="J50" s="25"/>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" s="5">
@@ -2489,37 +2524,39 @@
       <c r="C51" s="4">
         <v>5</v>
       </c>
-      <c r="D51" s="44" t="s">
+      <c r="D51" s="43" t="s">
         <v>108</v>
       </c>
-      <c r="E51" s="23">
+      <c r="E51" s="22">
         <v>44237</v>
       </c>
-      <c r="F51" s="89">
+      <c r="F51" s="87">
         <v>44617</v>
       </c>
-      <c r="G51" s="68" t="s">
+      <c r="G51" s="67" t="s">
         <v>105</v>
       </c>
       <c r="H51" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="I51" s="80"/>
-      <c r="J51" s="27"/>
+      <c r="I51" s="119" t="s">
+        <v>137</v>
+      </c>
+      <c r="J51" s="26"/>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" s="7"/>
       <c r="B52" s="6"/>
       <c r="C52" s="11"/>
-      <c r="D52" s="45"/>
-      <c r="E52" s="45"/>
-      <c r="F52" s="33"/>
-      <c r="G52" s="69">
+      <c r="D52" s="44"/>
+      <c r="E52" s="44"/>
+      <c r="F52" s="32"/>
+      <c r="G52" s="68">
         <v>89603906796</v>
       </c>
       <c r="H52" s="7"/>
-      <c r="I52" s="28"/>
-      <c r="J52" s="25"/>
+      <c r="I52" s="27"/>
+      <c r="J52" s="24"/>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" s="9"/>
@@ -2527,31 +2564,31 @@
       <c r="C53" s="12"/>
       <c r="D53" s="9"/>
       <c r="E53" s="9"/>
-      <c r="F53" s="46"/>
-      <c r="G53" s="70"/>
+      <c r="F53" s="45"/>
+      <c r="G53" s="69"/>
       <c r="H53" s="9"/>
-      <c r="I53" s="53"/>
-      <c r="J53" s="26"/>
-    </row>
-    <row r="55" spans="1:10" s="86" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I53" s="52"/>
+      <c r="J53" s="25"/>
+    </row>
+    <row r="55" spans="1:10" s="84" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
-      <c r="B55" s="87" t="s">
+      <c r="B55" s="85" t="s">
         <v>117</v>
       </c>
-      <c r="C55" s="88"/>
-      <c r="D55" s="88"/>
+      <c r="C55" s="86"/>
+      <c r="D55" s="86"/>
       <c r="E55" s="2"/>
-      <c r="F55" s="85"/>
-      <c r="G55" s="94" t="s">
+      <c r="F55" s="83"/>
+      <c r="G55" s="92" t="s">
         <v>125</v>
       </c>
-      <c r="H55" s="101"/>
-      <c r="I55" s="85"/>
-      <c r="J55" s="85"/>
-    </row>
-    <row r="56" spans="1:10" s="86" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H55" s="99"/>
+      <c r="I55" s="83"/>
+      <c r="J55" s="83"/>
+    </row>
+    <row r="56" spans="1:10" s="84" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="2"/>
-      <c r="B56" s="84" t="s">
+      <c r="B56" s="82" t="s">
         <v>113</v>
       </c>
       <c r="C56" s="2" t="s">
@@ -2559,19 +2596,19 @@
       </c>
       <c r="D56" s="2"/>
       <c r="E56" s="2"/>
-      <c r="F56" s="85"/>
-      <c r="G56" s="84" t="s">
+      <c r="F56" s="83"/>
+      <c r="G56" s="82" t="s">
         <v>109</v>
       </c>
       <c r="H56" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="I56" s="85"/>
-      <c r="J56" s="85"/>
-    </row>
-    <row r="57" spans="1:10" s="86" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I56" s="83"/>
+      <c r="J56" s="83"/>
+    </row>
+    <row r="57" spans="1:10" s="84" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
-      <c r="B57" s="84" t="s">
+      <c r="B57" s="82" t="s">
         <v>114</v>
       </c>
       <c r="C57" s="2" t="s">
@@ -2579,19 +2616,19 @@
       </c>
       <c r="D57" s="2"/>
       <c r="E57" s="2"/>
-      <c r="F57" s="85"/>
-      <c r="G57" s="84" t="s">
+      <c r="F57" s="83"/>
+      <c r="G57" s="82" t="s">
         <v>110</v>
       </c>
       <c r="H57" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="I57" s="85"/>
-      <c r="J57" s="85"/>
-    </row>
-    <row r="58" spans="1:10" s="86" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I57" s="83"/>
+      <c r="J57" s="83"/>
+    </row>
+    <row r="58" spans="1:10" s="84" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="2"/>
-      <c r="B58" s="84" t="s">
+      <c r="B58" s="82" t="s">
         <v>115</v>
       </c>
       <c r="C58" s="2" t="s">
@@ -2599,19 +2636,19 @@
       </c>
       <c r="D58" s="2"/>
       <c r="E58" s="2"/>
-      <c r="F58" s="85"/>
-      <c r="G58" s="84" t="s">
+      <c r="F58" s="83"/>
+      <c r="G58" s="82" t="s">
         <v>111</v>
       </c>
       <c r="H58" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="I58" s="85"/>
-      <c r="J58" s="85"/>
-    </row>
-    <row r="59" spans="1:10" s="86" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I58" s="83"/>
+      <c r="J58" s="83"/>
+    </row>
+    <row r="59" spans="1:10" s="84" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="2"/>
-      <c r="B59" s="84" t="s">
+      <c r="B59" s="82" t="s">
         <v>118</v>
       </c>
       <c r="C59" s="2" t="s">
@@ -2619,41 +2656,41 @@
       </c>
       <c r="D59" s="2"/>
       <c r="E59" s="2"/>
-      <c r="F59" s="85"/>
-      <c r="G59" s="84"/>
+      <c r="F59" s="83"/>
+      <c r="G59" s="82"/>
       <c r="H59" s="2"/>
-      <c r="I59" s="85"/>
-      <c r="J59" s="85"/>
-    </row>
-    <row r="60" spans="1:10" s="86" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I59" s="83"/>
+      <c r="J59" s="83"/>
+    </row>
+    <row r="60" spans="1:10" s="84" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
       <c r="D60" s="2"/>
       <c r="E60" s="2"/>
-      <c r="F60" s="85"/>
-      <c r="G60" s="84"/>
+      <c r="F60" s="83"/>
+      <c r="G60" s="82"/>
       <c r="H60" s="2"/>
-      <c r="I60" s="85"/>
-      <c r="J60" s="85"/>
-    </row>
-    <row r="61" spans="1:10" s="86" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I60" s="83"/>
+      <c r="J60" s="83"/>
+    </row>
+    <row r="61" spans="1:10" s="84" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="2"/>
-      <c r="B61" s="92" t="s">
+      <c r="B61" s="90" t="s">
         <v>124</v>
       </c>
-      <c r="C61" s="93"/>
+      <c r="C61" s="91"/>
       <c r="D61" s="2"/>
       <c r="E61" s="2"/>
-      <c r="F61" s="85"/>
-      <c r="G61" s="97" t="s">
+      <c r="F61" s="83"/>
+      <c r="G61" s="95" t="s">
         <v>128</v>
       </c>
-      <c r="H61" s="100"/>
-      <c r="I61" s="85"/>
-      <c r="J61" s="85"/>
-    </row>
-    <row r="62" spans="1:10" s="86" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H61" s="98"/>
+      <c r="I61" s="83"/>
+      <c r="J61" s="83"/>
+    </row>
+    <row r="62" spans="1:10" s="84" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="2"/>
-      <c r="B62" s="84" t="s">
+      <c r="B62" s="82" t="s">
         <v>119</v>
       </c>
       <c r="C62" s="2" t="s">
@@ -2661,19 +2698,19 @@
       </c>
       <c r="D62" s="2"/>
       <c r="E62" s="2"/>
-      <c r="F62" s="85"/>
-      <c r="G62" s="84" t="s">
+      <c r="F62" s="83"/>
+      <c r="G62" s="82" t="s">
         <v>126</v>
       </c>
       <c r="H62" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="I62" s="85"/>
-      <c r="J62" s="85"/>
-    </row>
-    <row r="63" spans="1:10" s="86" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I62" s="83"/>
+      <c r="J62" s="83"/>
+    </row>
+    <row r="63" spans="1:10" s="84" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="2"/>
-      <c r="B63" s="84" t="s">
+      <c r="B63" s="82" t="s">
         <v>120</v>
       </c>
       <c r="C63" s="2" t="s">
@@ -2681,15 +2718,15 @@
       </c>
       <c r="D63" s="2"/>
       <c r="E63" s="2"/>
-      <c r="F63" s="85"/>
-      <c r="G63" s="84"/>
+      <c r="F63" s="83"/>
+      <c r="G63" s="82"/>
       <c r="H63" s="2"/>
-      <c r="I63" s="85"/>
-      <c r="J63" s="85"/>
-    </row>
-    <row r="64" spans="1:10" s="86" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I63" s="83"/>
+      <c r="J63" s="83"/>
+    </row>
+    <row r="64" spans="1:10" s="84" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="2"/>
-      <c r="B64" s="84" t="s">
+      <c r="B64" s="82" t="s">
         <v>121</v>
       </c>
       <c r="C64" s="2" t="s">
@@ -2697,15 +2734,15 @@
       </c>
       <c r="D64" s="2"/>
       <c r="E64" s="2"/>
-      <c r="F64" s="85"/>
-      <c r="G64" s="84"/>
+      <c r="F64" s="83"/>
+      <c r="G64" s="82"/>
       <c r="H64" s="2"/>
-      <c r="I64" s="85"/>
-      <c r="J64" s="85"/>
-    </row>
-    <row r="65" spans="1:10" s="86" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I64" s="83"/>
+      <c r="J64" s="83"/>
+    </row>
+    <row r="65" spans="1:10" s="84" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="2"/>
-      <c r="B65" s="84" t="s">
+      <c r="B65" s="82" t="s">
         <v>122</v>
       </c>
       <c r="C65" s="2" t="s">
@@ -2713,11 +2750,11 @@
       </c>
       <c r="D65" s="2"/>
       <c r="E65" s="2"/>
-      <c r="F65" s="85"/>
-      <c r="G65" s="84"/>
+      <c r="F65" s="83"/>
+      <c r="G65" s="82"/>
       <c r="H65" s="2"/>
-      <c r="I65" s="85"/>
-      <c r="J65" s="85"/>
+      <c r="I65" s="83"/>
+      <c r="J65" s="83"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -2760,46 +2797,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="115" t="s">
+      <c r="A1" s="113" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="115" t="s">
+      <c r="B1" s="113" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="115" t="s">
+      <c r="C1" s="113" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="115" t="s">
+      <c r="D1" s="113" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="115"/>
-      <c r="F1" s="117" t="s">
+      <c r="E1" s="113"/>
+      <c r="F1" s="115" t="s">
         <v>106</v>
       </c>
-      <c r="G1" s="115" t="s">
+      <c r="G1" s="113" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="113" t="s">
+      <c r="H1" s="111" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="106" t="s">
+      <c r="I1" s="104" t="s">
         <v>56</v>
       </c>
-      <c r="J1" s="106"/>
+      <c r="J1" s="104"/>
     </row>
     <row r="2" spans="1:10" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="116"/>
-      <c r="B2" s="116"/>
-      <c r="C2" s="116"/>
-      <c r="D2" s="74" t="s">
+      <c r="A2" s="114"/>
+      <c r="B2" s="114"/>
+      <c r="C2" s="114"/>
+      <c r="D2" s="73" t="s">
         <v>6</v>
       </c>
       <c r="E2" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="118"/>
-      <c r="G2" s="116"/>
-      <c r="H2" s="114"/>
+      <c r="F2" s="116"/>
+      <c r="G2" s="114"/>
+      <c r="H2" s="112"/>
       <c r="I2" s="17" t="s">
         <v>6</v>
       </c>
@@ -2808,34 +2845,34 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="39">
+      <c r="A3" s="38">
         <v>1</v>
       </c>
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="40">
+      <c r="C3" s="39">
         <v>8</v>
       </c>
-      <c r="D3" s="58">
+      <c r="D3" s="57">
         <v>44218</v>
       </c>
-      <c r="E3" s="41" t="s">
+      <c r="E3" s="40" t="s">
         <v>84</v>
       </c>
-      <c r="F3" s="43" t="s">
+      <c r="F3" s="42" t="s">
         <v>87</v>
       </c>
-      <c r="G3" s="42" t="s">
+      <c r="G3" s="41" t="s">
         <v>85</v>
       </c>
-      <c r="H3" s="39" t="s">
+      <c r="H3" s="38" t="s">
         <v>89</v>
       </c>
-      <c r="I3" s="59">
+      <c r="I3" s="58">
         <v>44251</v>
       </c>
-      <c r="J3" s="61" t="s">
+      <c r="J3" s="60" t="s">
         <v>96</v>
       </c>
     </row>
@@ -2845,13 +2882,13 @@
       <c r="C4" s="11"/>
       <c r="D4" s="20"/>
       <c r="E4" s="20"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30">
+      <c r="F4" s="29"/>
+      <c r="G4" s="29">
         <v>85258844844</v>
       </c>
       <c r="H4" s="7"/>
-      <c r="I4" s="28"/>
-      <c r="J4" s="62"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="61"/>
     </row>
     <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9"/>
@@ -2859,11 +2896,11 @@
       <c r="C5" s="12"/>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="31"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
       <c r="H5" s="9"/>
-      <c r="I5" s="53"/>
-      <c r="J5" s="26"/>
+      <c r="I5" s="52"/>
+      <c r="J5" s="25"/>
     </row>
     <row r="6" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5">
@@ -2875,25 +2912,25 @@
       <c r="C6" s="4">
         <v>8</v>
       </c>
-      <c r="D6" s="44">
+      <c r="D6" s="43">
         <v>44218</v>
       </c>
       <c r="E6" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="F6" s="36" t="s">
+      <c r="F6" s="35" t="s">
         <v>87</v>
       </c>
-      <c r="G6" s="32" t="s">
+      <c r="G6" s="31" t="s">
         <v>86</v>
       </c>
       <c r="H6" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="I6" s="59">
+      <c r="I6" s="58">
         <v>44251</v>
       </c>
-      <c r="J6" s="56" t="s">
+      <c r="J6" s="55" t="s">
         <v>96</v>
       </c>
     </row>
@@ -2903,13 +2940,13 @@
       <c r="C7" s="11"/>
       <c r="D7" s="20"/>
       <c r="E7" s="20"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30">
+      <c r="F7" s="29"/>
+      <c r="G7" s="29">
         <v>82226183614</v>
       </c>
       <c r="H7" s="7"/>
-      <c r="I7" s="28"/>
-      <c r="J7" s="25"/>
+      <c r="I7" s="27"/>
+      <c r="J7" s="24"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="9"/>
@@ -2917,11 +2954,11 @@
       <c r="C8" s="12"/>
       <c r="D8" s="9"/>
       <c r="E8" s="9"/>
-      <c r="F8" s="31"/>
-      <c r="G8" s="31"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
       <c r="H8" s="9"/>
-      <c r="I8" s="53"/>
-      <c r="J8" s="26"/>
+      <c r="I8" s="52"/>
+      <c r="J8" s="25"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="7">
@@ -2936,22 +2973,22 @@
       <c r="D9" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="E9" s="63" t="s">
+      <c r="E9" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="35">
+      <c r="F9" s="34">
         <v>44440</v>
       </c>
-      <c r="G9" s="30" t="s">
+      <c r="G9" s="29" t="s">
         <v>90</v>
       </c>
       <c r="H9" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="I9" s="60" t="s">
+      <c r="I9" s="59" t="s">
         <v>95</v>
       </c>
-      <c r="J9" s="56" t="s">
+      <c r="J9" s="55" t="s">
         <v>96</v>
       </c>
     </row>
@@ -2961,13 +2998,13 @@
       <c r="C10" s="11"/>
       <c r="D10" s="7"/>
       <c r="E10" s="20"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30">
+      <c r="F10" s="29"/>
+      <c r="G10" s="29">
         <v>81232667763</v>
       </c>
       <c r="H10" s="7"/>
-      <c r="I10" s="28"/>
-      <c r="J10" s="25"/>
+      <c r="I10" s="27"/>
+      <c r="J10" s="24"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="7"/>
@@ -2975,11 +3012,11 @@
       <c r="C11" s="12"/>
       <c r="D11" s="9"/>
       <c r="E11" s="20"/>
-      <c r="F11" s="30"/>
-      <c r="G11" s="30"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="29"/>
       <c r="H11" s="7"/>
-      <c r="I11" s="28"/>
-      <c r="J11" s="25"/>
+      <c r="I11" s="27"/>
+      <c r="J11" s="24"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="7">
@@ -2994,22 +3031,22 @@
       <c r="D12" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="E12" s="63" t="s">
+      <c r="E12" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="F12" s="35">
+      <c r="F12" s="34">
         <v>44440</v>
       </c>
-      <c r="G12" s="30" t="s">
+      <c r="G12" s="29" t="s">
         <v>91</v>
       </c>
       <c r="H12" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="I12" s="60" t="s">
+      <c r="I12" s="59" t="s">
         <v>95</v>
       </c>
-      <c r="J12" s="56" t="s">
+      <c r="J12" s="55" t="s">
         <v>96</v>
       </c>
     </row>
@@ -3019,13 +3056,13 @@
       <c r="C13" s="11"/>
       <c r="D13" s="7"/>
       <c r="E13" s="20"/>
-      <c r="F13" s="30"/>
-      <c r="G13" s="30">
+      <c r="F13" s="29"/>
+      <c r="G13" s="29">
         <v>8214000800</v>
       </c>
       <c r="H13" s="7"/>
-      <c r="I13" s="28"/>
-      <c r="J13" s="25"/>
+      <c r="I13" s="27"/>
+      <c r="J13" s="24"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="7"/>
@@ -3033,14 +3070,14 @@
       <c r="C14" s="11"/>
       <c r="D14" s="7"/>
       <c r="E14" s="20"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="30"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="29"/>
       <c r="H14" s="7"/>
-      <c r="I14" s="28"/>
-      <c r="J14" s="25"/>
+      <c r="I14" s="27"/>
+      <c r="J14" s="24"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" s="24">
+      <c r="A15" s="23">
         <v>20</v>
       </c>
       <c r="B15" s="10" t="s">
@@ -3055,19 +3092,19 @@
       <c r="E15" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="F15" s="49" t="s">
+      <c r="F15" s="48" t="s">
         <v>63</v>
       </c>
-      <c r="G15" s="49" t="s">
+      <c r="G15" s="48" t="s">
         <v>37</v>
       </c>
       <c r="H15" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="I15" s="55">
+      <c r="I15" s="54">
         <v>44287</v>
       </c>
-      <c r="J15" s="56" t="s">
+      <c r="J15" s="55" t="s">
         <v>58</v>
       </c>
     </row>
@@ -3078,12 +3115,12 @@
       <c r="D16" s="20"/>
       <c r="E16" s="20"/>
       <c r="F16" s="15"/>
-      <c r="G16" s="50">
+      <c r="G16" s="49">
         <v>82170697118</v>
       </c>
       <c r="H16" s="15"/>
-      <c r="I16" s="28"/>
-      <c r="J16" s="25"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="24"/>
     </row>
     <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="9"/>
@@ -3092,40 +3129,40 @@
       <c r="D17" s="9"/>
       <c r="E17" s="9"/>
       <c r="F17" s="12"/>
-      <c r="G17" s="31"/>
+      <c r="G17" s="30"/>
       <c r="H17" s="12"/>
-      <c r="I17" s="53"/>
-      <c r="J17" s="26"/>
+      <c r="I17" s="52"/>
+      <c r="J17" s="25"/>
     </row>
     <row r="18" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="39">
+      <c r="A18" s="38">
         <v>3</v>
       </c>
-      <c r="B18" s="40" t="s">
+      <c r="B18" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="40">
+      <c r="C18" s="39">
         <v>9</v>
       </c>
-      <c r="D18" s="41" t="s">
+      <c r="D18" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="E18" s="41" t="s">
+      <c r="E18" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="F18" s="43">
+      <c r="F18" s="42">
         <v>44444</v>
       </c>
-      <c r="G18" s="64" t="s">
+      <c r="G18" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="H18" s="39" t="s">
+      <c r="H18" s="38" t="s">
         <v>66</v>
       </c>
-      <c r="I18" s="52" t="s">
+      <c r="I18" s="51" t="s">
         <v>53</v>
       </c>
-      <c r="J18" s="72" t="s">
+      <c r="J18" s="71" t="s">
         <v>98</v>
       </c>
     </row>
@@ -3135,13 +3172,13 @@
       <c r="C19" s="11"/>
       <c r="D19" s="20"/>
       <c r="E19" s="20"/>
-      <c r="F19" s="30"/>
-      <c r="G19" s="65">
+      <c r="F19" s="29"/>
+      <c r="G19" s="64">
         <v>81228196787</v>
       </c>
       <c r="H19" s="7"/>
-      <c r="I19" s="28"/>
-      <c r="J19" s="25"/>
+      <c r="I19" s="27"/>
+      <c r="J19" s="24"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="9"/>
@@ -3149,11 +3186,11 @@
       <c r="C20" s="12"/>
       <c r="D20" s="9"/>
       <c r="E20" s="9"/>
-      <c r="F20" s="31"/>
-      <c r="G20" s="66"/>
+      <c r="F20" s="30"/>
+      <c r="G20" s="65"/>
       <c r="H20" s="9"/>
-      <c r="I20" s="53"/>
-      <c r="J20" s="26"/>
+      <c r="I20" s="52"/>
+      <c r="J20" s="25"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="5">
@@ -3171,19 +3208,19 @@
       <c r="E21" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="F21" s="36">
+      <c r="F21" s="35">
         <v>44444</v>
       </c>
-      <c r="G21" s="67" t="s">
+      <c r="G21" s="66" t="s">
         <v>20</v>
       </c>
       <c r="H21" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="I21" s="54" t="s">
+      <c r="I21" s="53" t="s">
         <v>53</v>
       </c>
-      <c r="J21" s="72" t="s">
+      <c r="J21" s="71" t="s">
         <v>98</v>
       </c>
     </row>
@@ -3193,13 +3230,13 @@
       <c r="C22" s="11"/>
       <c r="D22" s="20"/>
       <c r="E22" s="20"/>
-      <c r="F22" s="30"/>
-      <c r="G22" s="65">
+      <c r="F22" s="29"/>
+      <c r="G22" s="64">
         <v>81225736355</v>
       </c>
       <c r="H22" s="7"/>
-      <c r="I22" s="28"/>
-      <c r="J22" s="25"/>
+      <c r="I22" s="27"/>
+      <c r="J22" s="24"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="9"/>
@@ -3207,14 +3244,14 @@
       <c r="C23" s="12"/>
       <c r="D23" s="9"/>
       <c r="E23" s="9"/>
-      <c r="F23" s="31"/>
-      <c r="G23" s="66"/>
+      <c r="F23" s="30"/>
+      <c r="G23" s="65"/>
       <c r="H23" s="9"/>
-      <c r="I23" s="53"/>
-      <c r="J23" s="26"/>
+      <c r="I23" s="52"/>
+      <c r="J23" s="25"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A24" s="24">
+      <c r="A24" s="23">
         <v>13</v>
       </c>
       <c r="B24" s="10" t="s">
@@ -3223,25 +3260,25 @@
       <c r="C24" s="10">
         <v>30</v>
       </c>
-      <c r="D24" s="44">
+      <c r="D24" s="43">
         <v>44253</v>
       </c>
-      <c r="E24" s="44" t="s">
+      <c r="E24" s="43" t="s">
         <v>54</v>
       </c>
-      <c r="F24" s="32" t="s">
+      <c r="F24" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="G24" s="67" t="s">
+      <c r="G24" s="66" t="s">
         <v>34</v>
       </c>
-      <c r="H24" s="24" t="s">
+      <c r="H24" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="I24" s="55">
+      <c r="I24" s="54">
         <v>44287</v>
       </c>
-      <c r="J24" s="72" t="s">
+      <c r="J24" s="71" t="s">
         <v>98</v>
       </c>
     </row>
@@ -3251,25 +3288,25 @@
       <c r="C25" s="15"/>
       <c r="D25" s="20"/>
       <c r="E25" s="20"/>
-      <c r="F25" s="30"/>
-      <c r="G25" s="65">
+      <c r="F25" s="29"/>
+      <c r="G25" s="64">
         <v>82110632173</v>
       </c>
       <c r="H25" s="20"/>
-      <c r="I25" s="28"/>
-      <c r="J25" s="25"/>
+      <c r="I25" s="27"/>
+      <c r="J25" s="24"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A26" s="22"/>
+      <c r="A26" s="21"/>
       <c r="B26" s="16"/>
       <c r="C26" s="16"/>
       <c r="D26" s="9"/>
       <c r="E26" s="9"/>
-      <c r="F26" s="31"/>
-      <c r="G26" s="66"/>
-      <c r="H26" s="22"/>
-      <c r="I26" s="53"/>
-      <c r="J26" s="26"/>
+      <c r="F26" s="30"/>
+      <c r="G26" s="65"/>
+      <c r="H26" s="21"/>
+      <c r="I26" s="52"/>
+      <c r="J26" s="25"/>
     </row>
     <row r="27" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="5">
@@ -3287,19 +3324,19 @@
       <c r="E27" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="F27" s="32" t="s">
+      <c r="F27" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="G27" s="67" t="s">
+      <c r="G27" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="H27" s="24" t="s">
+      <c r="H27" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="I27" s="54" t="s">
+      <c r="I27" s="53" t="s">
         <v>53</v>
       </c>
-      <c r="J27" s="72" t="s">
+      <c r="J27" s="71" t="s">
         <v>98</v>
       </c>
     </row>
@@ -3309,13 +3346,13 @@
       <c r="C28" s="15"/>
       <c r="D28" s="7"/>
       <c r="E28" s="20"/>
-      <c r="F28" s="30"/>
-      <c r="G28" s="65">
+      <c r="F28" s="29"/>
+      <c r="G28" s="64">
         <v>81231558203</v>
       </c>
       <c r="H28" s="20"/>
-      <c r="I28" s="28"/>
-      <c r="J28" s="25"/>
+      <c r="I28" s="27"/>
+      <c r="J28" s="24"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="9"/>
@@ -3323,11 +3360,11 @@
       <c r="C29" s="16"/>
       <c r="D29" s="9"/>
       <c r="E29" s="9"/>
-      <c r="F29" s="31"/>
-      <c r="G29" s="66"/>
-      <c r="H29" s="22"/>
-      <c r="I29" s="53"/>
-      <c r="J29" s="26"/>
+      <c r="F29" s="30"/>
+      <c r="G29" s="65"/>
+      <c r="H29" s="21"/>
+      <c r="I29" s="52"/>
+      <c r="J29" s="25"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="7">
@@ -3339,25 +3376,25 @@
       <c r="C30" s="10">
         <v>38</v>
       </c>
-      <c r="D30" s="44">
+      <c r="D30" s="43">
         <v>44253</v>
       </c>
       <c r="E30" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="F30" s="32" t="s">
+      <c r="F30" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="G30" s="67" t="s">
+      <c r="G30" s="66" t="s">
         <v>36</v>
       </c>
-      <c r="H30" s="24" t="s">
+      <c r="H30" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="I30" s="55">
+      <c r="I30" s="54">
         <v>44246</v>
       </c>
-      <c r="J30" s="72" t="s">
+      <c r="J30" s="71" t="s">
         <v>98</v>
       </c>
     </row>
@@ -3367,25 +3404,25 @@
       <c r="C31" s="15"/>
       <c r="D31" s="6"/>
       <c r="E31" s="20"/>
-      <c r="F31" s="30"/>
-      <c r="G31" s="65">
+      <c r="F31" s="29"/>
+      <c r="G31" s="64">
         <v>81318154783</v>
       </c>
       <c r="H31" s="20"/>
-      <c r="I31" s="28"/>
-      <c r="J31" s="25"/>
+      <c r="I31" s="27"/>
+      <c r="J31" s="24"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="7"/>
-      <c r="B32" s="51"/>
-      <c r="C32" s="51"/>
+      <c r="B32" s="50"/>
+      <c r="C32" s="50"/>
       <c r="D32" s="9"/>
       <c r="E32" s="9"/>
-      <c r="F32" s="31"/>
-      <c r="G32" s="66"/>
-      <c r="H32" s="22"/>
-      <c r="I32" s="26"/>
-      <c r="J32" s="26"/>
+      <c r="F32" s="30"/>
+      <c r="G32" s="65"/>
+      <c r="H32" s="21"/>
+      <c r="I32" s="25"/>
+      <c r="J32" s="25"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="5">
@@ -3397,25 +3434,25 @@
       <c r="C33" s="10">
         <v>38</v>
       </c>
-      <c r="D33" s="44">
+      <c r="D33" s="43">
         <v>44253</v>
       </c>
       <c r="E33" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="F33" s="32" t="s">
+      <c r="F33" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="G33" s="67" t="s">
+      <c r="G33" s="66" t="s">
         <v>38</v>
       </c>
-      <c r="H33" s="24" t="s">
+      <c r="H33" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="I33" s="55">
+      <c r="I33" s="54">
         <v>44246</v>
       </c>
-      <c r="J33" s="72" t="s">
+      <c r="J33" s="71" t="s">
         <v>98</v>
       </c>
     </row>
@@ -3425,25 +3462,25 @@
       <c r="C34" s="15"/>
       <c r="D34" s="6"/>
       <c r="E34" s="20"/>
-      <c r="F34" s="30"/>
-      <c r="G34" s="65">
+      <c r="F34" s="29"/>
+      <c r="G34" s="64">
         <v>8123929482</v>
       </c>
       <c r="H34" s="20"/>
-      <c r="I34" s="28"/>
-      <c r="J34" s="25"/>
+      <c r="I34" s="27"/>
+      <c r="J34" s="24"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="9"/>
-      <c r="B35" s="51"/>
-      <c r="C35" s="51"/>
+      <c r="B35" s="50"/>
+      <c r="C35" s="50"/>
       <c r="D35" s="9"/>
       <c r="E35" s="9"/>
-      <c r="F35" s="31"/>
-      <c r="G35" s="66"/>
-      <c r="H35" s="22"/>
-      <c r="I35" s="26"/>
-      <c r="J35" s="26"/>
+      <c r="F35" s="30"/>
+      <c r="G35" s="65"/>
+      <c r="H35" s="21"/>
+      <c r="I35" s="25"/>
+      <c r="J35" s="25"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="7">
@@ -3461,19 +3498,19 @@
       <c r="E36" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="F36" s="36">
+      <c r="F36" s="35">
         <v>44444</v>
       </c>
-      <c r="G36" s="67" t="s">
+      <c r="G36" s="66" t="s">
         <v>25</v>
       </c>
       <c r="H36" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="I36" s="54" t="s">
+      <c r="I36" s="53" t="s">
         <v>53</v>
       </c>
-      <c r="J36" s="72" t="s">
+      <c r="J36" s="71" t="s">
         <v>98</v>
       </c>
     </row>
@@ -3483,13 +3520,13 @@
       <c r="C37" s="11"/>
       <c r="D37" s="7"/>
       <c r="E37" s="7"/>
-      <c r="F37" s="30"/>
-      <c r="G37" s="65">
+      <c r="F37" s="29"/>
+      <c r="G37" s="64">
         <v>81331414130</v>
       </c>
       <c r="H37" s="7"/>
-      <c r="I37" s="25"/>
-      <c r="J37" s="25"/>
+      <c r="I37" s="24"/>
+      <c r="J37" s="24"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="7"/>
@@ -3497,11 +3534,11 @@
       <c r="C38" s="12"/>
       <c r="D38" s="9"/>
       <c r="E38" s="9"/>
-      <c r="F38" s="31"/>
-      <c r="G38" s="66"/>
+      <c r="F38" s="30"/>
+      <c r="G38" s="65"/>
       <c r="H38" s="9"/>
-      <c r="I38" s="26"/>
-      <c r="J38" s="26"/>
+      <c r="I38" s="25"/>
+      <c r="J38" s="25"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="5">
@@ -3519,19 +3556,19 @@
       <c r="E39" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="F39" s="36">
+      <c r="F39" s="35">
         <v>44444</v>
       </c>
-      <c r="G39" s="67" t="s">
+      <c r="G39" s="66" t="s">
         <v>26</v>
       </c>
       <c r="H39" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="I39" s="54" t="s">
+      <c r="I39" s="53" t="s">
         <v>53</v>
       </c>
-      <c r="J39" s="72" t="s">
+      <c r="J39" s="71" t="s">
         <v>98</v>
       </c>
     </row>
@@ -3541,13 +3578,13 @@
       <c r="C40" s="11"/>
       <c r="D40" s="7"/>
       <c r="E40" s="7"/>
-      <c r="F40" s="30"/>
-      <c r="G40" s="65">
+      <c r="F40" s="29"/>
+      <c r="G40" s="64">
         <v>81252283477</v>
       </c>
       <c r="H40" s="7"/>
-      <c r="I40" s="25"/>
-      <c r="J40" s="25"/>
+      <c r="I40" s="24"/>
+      <c r="J40" s="24"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="9"/>
@@ -3555,11 +3592,11 @@
       <c r="C41" s="12"/>
       <c r="D41" s="9"/>
       <c r="E41" s="9"/>
-      <c r="F41" s="31"/>
-      <c r="G41" s="66"/>
+      <c r="F41" s="30"/>
+      <c r="G41" s="65"/>
       <c r="H41" s="9"/>
-      <c r="I41" s="26"/>
-      <c r="J41" s="26"/>
+      <c r="I41" s="25"/>
+      <c r="J41" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>

<commit_message>
ukur 25 okt 2021
</commit_message>
<xml_diff>
--- a/RENCANA BON VOYAGE.xlsx
+++ b/RENCANA BON VOYAGE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mapan\progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5235210C-EE7D-4992-BA3A-4FA7DB6D8649}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F953EED-34F1-46B2-A372-8B77BFF91B56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="150">
   <si>
     <t>NO</t>
   </si>
@@ -469,6 +469,12 @@
   </si>
   <si>
     <t>01 MARET</t>
+  </si>
+  <si>
+    <t>HAMSAH</t>
+  </si>
+  <si>
+    <t>081234803574</t>
   </si>
 </sst>
 </file>
@@ -615,7 +621,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="141">
+  <cellXfs count="142">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -926,45 +932,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1022,6 +989,48 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1727,8 +1736,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:J84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="G65" sqref="G65"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1747,46 +1756,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="108" t="s">
+      <c r="A1" s="128" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="108" t="s">
+      <c r="B1" s="128" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="108" t="s">
+      <c r="C1" s="128" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="114" t="s">
+      <c r="D1" s="134" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="114"/>
-      <c r="F1" s="112" t="s">
+      <c r="E1" s="134"/>
+      <c r="F1" s="132" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="110" t="s">
+      <c r="G1" s="130" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="108" t="s">
+      <c r="H1" s="128" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="108" t="s">
+      <c r="I1" s="128" t="s">
         <v>56</v>
       </c>
-      <c r="J1" s="108"/>
+      <c r="J1" s="128"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="109"/>
-      <c r="B2" s="109"/>
-      <c r="C2" s="109"/>
+      <c r="A2" s="129"/>
+      <c r="B2" s="129"/>
+      <c r="C2" s="129"/>
       <c r="D2" s="17" t="s">
         <v>6</v>
       </c>
       <c r="E2" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="113"/>
-      <c r="G2" s="111"/>
-      <c r="H2" s="109"/>
+      <c r="F2" s="133"/>
+      <c r="G2" s="131"/>
+      <c r="H2" s="129"/>
       <c r="I2" s="17" t="s">
         <v>6</v>
       </c>
@@ -2142,16 +2151,16 @@
       <c r="C21" s="4">
         <v>18</v>
       </c>
-      <c r="D21" s="121" t="s">
+      <c r="D21" s="108" t="s">
         <v>141</v>
       </c>
       <c r="E21" s="97" t="s">
         <v>143</v>
       </c>
-      <c r="F21" s="127" t="s">
+      <c r="F21" s="114" t="s">
         <v>142</v>
       </c>
-      <c r="G21" s="122"/>
+      <c r="G21" s="109"/>
       <c r="H21" s="23"/>
       <c r="I21" s="78"/>
       <c r="J21" s="26"/>
@@ -2162,8 +2171,8 @@
       <c r="C22" s="11"/>
       <c r="D22" s="36"/>
       <c r="E22" s="36"/>
-      <c r="F22" s="123"/>
-      <c r="G22" s="124"/>
+      <c r="F22" s="110"/>
+      <c r="G22" s="111"/>
       <c r="H22" s="20"/>
       <c r="I22" s="102"/>
       <c r="J22" s="24"/>
@@ -2174,8 +2183,8 @@
       <c r="C23" s="12"/>
       <c r="D23" s="21"/>
       <c r="E23" s="21"/>
-      <c r="F23" s="125"/>
-      <c r="G23" s="126"/>
+      <c r="F23" s="112"/>
+      <c r="G23" s="113"/>
       <c r="H23" s="21"/>
       <c r="I23" s="103"/>
       <c r="J23" s="25"/>
@@ -2190,14 +2199,16 @@
       <c r="C24" s="4">
         <v>18</v>
       </c>
-      <c r="D24" s="121"/>
+      <c r="D24" s="108"/>
       <c r="E24" s="97" t="s">
         <v>143</v>
       </c>
-      <c r="F24" s="127" t="s">
+      <c r="F24" s="114" t="s">
         <v>142</v>
       </c>
-      <c r="G24" s="122"/>
+      <c r="G24" s="109" t="s">
+        <v>148</v>
+      </c>
       <c r="H24" s="23"/>
       <c r="I24" s="78"/>
       <c r="J24" s="26"/>
@@ -2208,8 +2219,10 @@
       <c r="C25" s="11"/>
       <c r="D25" s="36"/>
       <c r="E25" s="36"/>
-      <c r="F25" s="123"/>
-      <c r="G25" s="124"/>
+      <c r="F25" s="110"/>
+      <c r="G25" s="141" t="s">
+        <v>149</v>
+      </c>
       <c r="H25" s="20"/>
       <c r="I25" s="102"/>
       <c r="J25" s="24"/>
@@ -2220,8 +2233,8 @@
       <c r="C26" s="12"/>
       <c r="D26" s="21"/>
       <c r="E26" s="21"/>
-      <c r="F26" s="125"/>
-      <c r="G26" s="126"/>
+      <c r="F26" s="112"/>
+      <c r="G26" s="113"/>
       <c r="H26" s="21"/>
       <c r="I26" s="103"/>
       <c r="J26" s="25"/>
@@ -2720,7 +2733,7 @@
       <c r="I53" s="52"/>
       <c r="J53" s="25"/>
     </row>
-    <row r="54" spans="1:10" s="131" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:10" s="118" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A54" s="5">
         <v>18</v>
       </c>
@@ -2734,37 +2747,37 @@
       <c r="E54" s="74" t="s">
         <v>145</v>
       </c>
-      <c r="F54" s="138" t="s">
+      <c r="F54" s="125" t="s">
         <v>144</v>
       </c>
-      <c r="G54" s="129"/>
+      <c r="G54" s="116"/>
       <c r="H54" s="23"/>
       <c r="I54" s="78"/>
-      <c r="J54" s="130"/>
-    </row>
-    <row r="55" spans="1:10" s="131" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J54" s="117"/>
+    </row>
+    <row r="55" spans="1:10" s="118" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A55" s="7"/>
       <c r="B55" s="102"/>
       <c r="C55" s="15"/>
       <c r="D55" s="36"/>
       <c r="E55" s="36"/>
-      <c r="F55" s="132"/>
-      <c r="G55" s="133"/>
+      <c r="F55" s="119"/>
+      <c r="G55" s="120"/>
       <c r="H55" s="20"/>
       <c r="I55" s="102"/>
-      <c r="J55" s="134"/>
-    </row>
-    <row r="56" spans="1:10" s="131" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J55" s="121"/>
+    </row>
+    <row r="56" spans="1:10" s="118" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="9"/>
       <c r="B56" s="103"/>
       <c r="C56" s="16"/>
       <c r="D56" s="21"/>
       <c r="E56" s="21"/>
-      <c r="F56" s="135"/>
-      <c r="G56" s="136"/>
+      <c r="F56" s="122"/>
+      <c r="G56" s="123"/>
       <c r="H56" s="21"/>
       <c r="I56" s="103"/>
-      <c r="J56" s="137"/>
+      <c r="J56" s="124"/>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57" s="5">
@@ -2888,16 +2901,16 @@
       <c r="C63" s="10">
         <v>41</v>
       </c>
-      <c r="D63" s="139"/>
+      <c r="D63" s="126"/>
       <c r="E63" s="74" t="s">
         <v>147</v>
       </c>
-      <c r="F63" s="128" t="s">
+      <c r="F63" s="115" t="s">
         <v>146</v>
       </c>
-      <c r="G63" s="129"/>
+      <c r="G63" s="116"/>
       <c r="H63" s="23"/>
-      <c r="I63" s="140"/>
+      <c r="I63" s="127"/>
       <c r="J63" s="26"/>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.2">
@@ -2906,8 +2919,8 @@
       <c r="C64" s="15"/>
       <c r="D64" s="36"/>
       <c r="E64" s="36"/>
-      <c r="F64" s="132"/>
-      <c r="G64" s="133"/>
+      <c r="F64" s="119"/>
+      <c r="G64" s="120"/>
       <c r="H64" s="20"/>
       <c r="I64" s="102"/>
       <c r="J64" s="24"/>
@@ -2918,8 +2931,8 @@
       <c r="C65" s="16"/>
       <c r="D65" s="21"/>
       <c r="E65" s="21"/>
-      <c r="F65" s="135"/>
-      <c r="G65" s="136"/>
+      <c r="F65" s="122"/>
+      <c r="G65" s="123"/>
       <c r="H65" s="21"/>
       <c r="I65" s="103"/>
       <c r="J65" s="25"/>
@@ -2934,16 +2947,16 @@
       <c r="C66" s="10">
         <v>41</v>
       </c>
-      <c r="D66" s="139"/>
+      <c r="D66" s="126"/>
       <c r="E66" s="74" t="s">
         <v>147</v>
       </c>
-      <c r="F66" s="128" t="s">
+      <c r="F66" s="115" t="s">
         <v>146</v>
       </c>
-      <c r="G66" s="129"/>
+      <c r="G66" s="116"/>
       <c r="H66" s="23"/>
-      <c r="I66" s="140"/>
+      <c r="I66" s="127"/>
       <c r="J66" s="26"/>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.2">
@@ -2952,8 +2965,8 @@
       <c r="C67" s="15"/>
       <c r="D67" s="36"/>
       <c r="E67" s="36"/>
-      <c r="F67" s="132"/>
-      <c r="G67" s="133"/>
+      <c r="F67" s="119"/>
+      <c r="G67" s="120"/>
       <c r="H67" s="20"/>
       <c r="I67" s="102"/>
       <c r="J67" s="24"/>
@@ -2964,8 +2977,8 @@
       <c r="C68" s="16"/>
       <c r="D68" s="21"/>
       <c r="E68" s="21"/>
-      <c r="F68" s="135"/>
-      <c r="G68" s="136"/>
+      <c r="F68" s="122"/>
+      <c r="G68" s="123"/>
       <c r="H68" s="21"/>
       <c r="I68" s="103"/>
       <c r="J68" s="25"/>
@@ -3258,46 +3271,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="117" t="s">
+      <c r="A1" s="137" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="117" t="s">
+      <c r="B1" s="137" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="117" t="s">
+      <c r="C1" s="137" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="117" t="s">
+      <c r="D1" s="137" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="117"/>
-      <c r="F1" s="119" t="s">
+      <c r="E1" s="137"/>
+      <c r="F1" s="139" t="s">
         <v>106</v>
       </c>
-      <c r="G1" s="117" t="s">
+      <c r="G1" s="137" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="115" t="s">
+      <c r="H1" s="135" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="108" t="s">
+      <c r="I1" s="128" t="s">
         <v>56</v>
       </c>
-      <c r="J1" s="108"/>
+      <c r="J1" s="128"/>
     </row>
     <row r="2" spans="1:10" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="118"/>
-      <c r="B2" s="118"/>
-      <c r="C2" s="118"/>
+      <c r="A2" s="138"/>
+      <c r="B2" s="138"/>
+      <c r="C2" s="138"/>
       <c r="D2" s="73" t="s">
         <v>6</v>
       </c>
       <c r="E2" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="120"/>
-      <c r="G2" s="118"/>
-      <c r="H2" s="116"/>
+      <c r="F2" s="140"/>
+      <c r="G2" s="138"/>
+      <c r="H2" s="136"/>
       <c r="I2" s="17" t="s">
         <v>6</v>
       </c>

</xml_diff>